<commit_message>
Added dockerfile, larger IDFT images, still searching for ideal beta
</commit_message>
<xml_diff>
--- a/beta_bruteforce.xlsx
+++ b/beta_bruteforce.xlsx
@@ -527,2242 +527,2242 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.001</v>
+        <v>0.1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6916699418272468</v>
+        <v>0.8566587236151254</v>
       </c>
       <c r="C2" t="n">
-        <v>1.744784384616679</v>
+        <v>1.771187517673625</v>
       </c>
       <c r="D2" t="n">
-        <v>3.163739630461398</v>
+        <v>2.147256901232214</v>
       </c>
       <c r="E2" t="n">
-        <v>3.319026832918979</v>
+        <v>3.555792545954183</v>
       </c>
       <c r="F2" t="n">
-        <v>2.920005516447551</v>
+        <v>3.269734193299858</v>
       </c>
       <c r="G2" t="n">
-        <v>2.129078450484733</v>
+        <v>3.097999695339084</v>
       </c>
       <c r="H2" t="n">
-        <v>2.320423694139823</v>
+        <v>2.667483306975116</v>
       </c>
       <c r="I2" t="n">
-        <v>1.915701365639154</v>
+        <v>1.871130384184854</v>
       </c>
       <c r="J2" t="n">
-        <v>1.771021019060541</v>
+        <v>1.810626526673194</v>
       </c>
       <c r="K2" t="n">
-        <v>1.820117171110034</v>
+        <v>1.724899721617806</v>
       </c>
       <c r="L2" t="n">
-        <v>1.812949878444037</v>
+        <v>1.540870981385511</v>
       </c>
       <c r="M2" t="n">
-        <v>1.809536712337378</v>
+        <v>1.473634073900036</v>
       </c>
       <c r="N2" t="n">
-        <v>1.797593981740846</v>
+        <v>1.460618899975976</v>
       </c>
       <c r="O2" t="n">
-        <v>1.787413749992918</v>
+        <v>1.454465072202204</v>
       </c>
       <c r="P2" t="n">
-        <v>1.775332152591644</v>
+        <v>1.461266851839339</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.773236095608555</v>
+        <v>1.459377401762835</v>
       </c>
       <c r="R2" t="n">
-        <v>1.771349057861555</v>
+        <v>1.449071767183183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.0013433993325989</v>
+        <v>0.1244071624980818</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6911960151651327</v>
+        <v>0.8351626818621439</v>
       </c>
       <c r="C3" t="n">
-        <v>1.746305984519982</v>
+        <v>1.60531946353026</v>
       </c>
       <c r="D3" t="n">
-        <v>3.13479998533274</v>
+        <v>1.888863534345361</v>
       </c>
       <c r="E3" t="n">
-        <v>3.226875017585412</v>
+        <v>3.391276799669774</v>
       </c>
       <c r="F3" t="n">
-        <v>2.921112529965102</v>
+        <v>3.118603389223044</v>
       </c>
       <c r="G3" t="n">
-        <v>2.102168907155666</v>
+        <v>2.957605134094258</v>
       </c>
       <c r="H3" t="n">
-        <v>2.309600173303942</v>
+        <v>2.590792625638696</v>
       </c>
       <c r="I3" t="n">
-        <v>1.896276512699347</v>
+        <v>1.837124333888601</v>
       </c>
       <c r="J3" t="n">
-        <v>1.736514252707721</v>
+        <v>1.735716535868425</v>
       </c>
       <c r="K3" t="n">
-        <v>1.739776476452368</v>
+        <v>1.675023276314817</v>
       </c>
       <c r="L3" t="n">
-        <v>1.734247181000541</v>
+        <v>1.496945805633497</v>
       </c>
       <c r="M3" t="n">
-        <v>1.726756545699387</v>
+        <v>1.422669116387521</v>
       </c>
       <c r="N3" t="n">
-        <v>1.711036669010266</v>
+        <v>1.399940817116471</v>
       </c>
       <c r="O3" t="n">
-        <v>1.699004654343549</v>
+        <v>1.386097822898307</v>
       </c>
       <c r="P3" t="n">
-        <v>1.686030760519</v>
+        <v>1.390069131331246</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.683689339376308</v>
+        <v>1.386383039640563</v>
       </c>
       <c r="R3" t="n">
-        <v>1.67854230731971</v>
+        <v>1.375167143214053</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.00180472176682717</v>
+        <v>0.1547714208082412</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6905765687734787</v>
+        <v>0.812628678457862</v>
       </c>
       <c r="C4" t="n">
-        <v>1.746388304743996</v>
+        <v>1.418756154944647</v>
       </c>
       <c r="D4" t="n">
-        <v>3.101470265876055</v>
+        <v>1.695287182784697</v>
       </c>
       <c r="E4" t="n">
-        <v>3.120609222940844</v>
+        <v>3.146055706776008</v>
       </c>
       <c r="F4" t="n">
-        <v>2.924766873689783</v>
+        <v>2.950644735566587</v>
       </c>
       <c r="G4" t="n">
-        <v>2.078654819506041</v>
+        <v>2.803113550587407</v>
       </c>
       <c r="H4" t="n">
-        <v>2.29301988849074</v>
+        <v>2.50457689307441</v>
       </c>
       <c r="I4" t="n">
-        <v>1.873161937221181</v>
+        <v>1.788794974265002</v>
       </c>
       <c r="J4" t="n">
-        <v>1.695039481343533</v>
+        <v>1.648982537543726</v>
       </c>
       <c r="K4" t="n">
-        <v>1.707394879389103</v>
+        <v>1.613044311885958</v>
       </c>
       <c r="L4" t="n">
-        <v>1.64852717329154</v>
+        <v>1.443152506968225</v>
       </c>
       <c r="M4" t="n">
-        <v>1.637105384602354</v>
+        <v>1.362660005557402</v>
       </c>
       <c r="N4" t="n">
-        <v>1.616730482459988</v>
+        <v>1.330287458642536</v>
       </c>
       <c r="O4" t="n">
-        <v>1.602800038388563</v>
+        <v>1.308636403134852</v>
       </c>
       <c r="P4" t="n">
-        <v>1.606865225599921</v>
+        <v>1.309250029099277</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.619086071127566</v>
+        <v>1.303100627163071</v>
       </c>
       <c r="R4" t="n">
-        <v>1.606778970689145</v>
+        <v>1.296841035686678</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.002424462017082328</v>
+        <v>0.1925467329854986</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6897521634686548</v>
+        <v>0.7890149522074585</v>
       </c>
       <c r="C5" t="n">
-        <v>1.744113656115166</v>
+        <v>1.212420271394019</v>
       </c>
       <c r="D5" t="n">
-        <v>3.062412458188729</v>
+        <v>1.575597851661433</v>
       </c>
       <c r="E5" t="n">
-        <v>2.999081772242882</v>
+        <v>2.888156935813938</v>
       </c>
       <c r="F5" t="n">
-        <v>2.93135249525116</v>
+        <v>2.766246997015567</v>
       </c>
       <c r="G5" t="n">
-        <v>2.058277671044888</v>
+        <v>2.640435127908572</v>
       </c>
       <c r="H5" t="n">
-        <v>2.270129884323057</v>
+        <v>2.408707157528997</v>
       </c>
       <c r="I5" t="n">
-        <v>1.859274440032493</v>
+        <v>1.810120497347106</v>
       </c>
       <c r="J5" t="n">
-        <v>1.645952617628944</v>
+        <v>1.613718472517327</v>
       </c>
       <c r="K5" t="n">
-        <v>1.663847407584672</v>
+        <v>1.538377114359197</v>
       </c>
       <c r="L5" t="n">
-        <v>1.639526429142606</v>
+        <v>1.379298014255225</v>
       </c>
       <c r="M5" t="n">
-        <v>1.621697079379939</v>
+        <v>1.293839625327438</v>
       </c>
       <c r="N5" t="n">
-        <v>1.595481246311532</v>
+        <v>1.252229187735173</v>
       </c>
       <c r="O5" t="n">
-        <v>1.586380478029517</v>
+        <v>1.24335425874434</v>
       </c>
       <c r="P5" t="n">
-        <v>1.565678847669234</v>
+        <v>1.268116474543026</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.573412757462377</v>
+        <v>1.286511208075842</v>
       </c>
       <c r="R5" t="n">
-        <v>1.566496590469795</v>
+        <v>1.294384692940456</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.003257020655659783</v>
+        <v>0.2395419269900167</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6886573980506793</v>
+        <v>0.7642764190735251</v>
       </c>
       <c r="C6" t="n">
-        <v>1.738171849138135</v>
+        <v>1.150433961656988</v>
       </c>
       <c r="D6" t="n">
-        <v>3.015659733974354</v>
+        <v>1.439607451843186</v>
       </c>
       <c r="E6" t="n">
-        <v>2.860861348082169</v>
+        <v>2.618787531968784</v>
       </c>
       <c r="F6" t="n">
-        <v>2.940847484367062</v>
+        <v>2.566090784825579</v>
       </c>
       <c r="G6" t="n">
-        <v>2.073780976440652</v>
+        <v>2.480015430347491</v>
       </c>
       <c r="H6" t="n">
-        <v>2.280634084238041</v>
+        <v>2.303358932074378</v>
       </c>
       <c r="I6" t="n">
-        <v>1.847346168405207</v>
+        <v>1.816000894670207</v>
       </c>
       <c r="J6" t="n">
-        <v>1.659796692419616</v>
+        <v>1.621729918752989</v>
       </c>
       <c r="K6" t="n">
-        <v>1.608721205952561</v>
+        <v>1.450860828413764</v>
       </c>
       <c r="L6" t="n">
-        <v>1.645603958366457</v>
+        <v>1.305464387623296</v>
       </c>
       <c r="M6" t="n">
-        <v>1.635158472601985</v>
+        <v>1.287396664493389</v>
       </c>
       <c r="N6" t="n">
-        <v>1.612219019506677</v>
+        <v>1.233844774616363</v>
       </c>
       <c r="O6" t="n">
-        <v>1.596053024987508</v>
+        <v>1.232927857633659</v>
       </c>
       <c r="P6" t="n">
-        <v>1.565317342995477</v>
+        <v>1.251704440018779</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.545011343606597</v>
+        <v>1.265834089542243</v>
       </c>
       <c r="R6" t="n">
-        <v>1.525585525331923</v>
+        <v>1.268567990960848</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.004375479375074184</v>
+        <v>0.2980073143615066</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6872017370926496</v>
+        <v>0.7384188825332056</v>
       </c>
       <c r="C7" t="n">
-        <v>1.726798487037097</v>
+        <v>1.085738632244158</v>
       </c>
       <c r="D7" t="n">
-        <v>2.958662618047696</v>
+        <v>1.286978855225746</v>
       </c>
       <c r="E7" t="n">
-        <v>2.803437384283877</v>
+        <v>2.339487680255643</v>
       </c>
       <c r="F7" t="n">
-        <v>2.952747902314125</v>
+        <v>2.351155505797511</v>
       </c>
       <c r="G7" t="n">
-        <v>2.099405652242347</v>
+        <v>2.298213367466672</v>
       </c>
       <c r="H7" t="n">
-        <v>2.28612664529282</v>
+        <v>2.189007743144729</v>
       </c>
       <c r="I7" t="n">
-        <v>1.832309411223711</v>
+        <v>1.7987700669252</v>
       </c>
       <c r="J7" t="n">
-        <v>1.681364376469016</v>
+        <v>1.605926226632588</v>
       </c>
       <c r="K7" t="n">
-        <v>1.542259589822613</v>
+        <v>1.435341853533926</v>
       </c>
       <c r="L7" t="n">
-        <v>1.646440682578343</v>
+        <v>1.284222686069711</v>
       </c>
       <c r="M7" t="n">
-        <v>1.64446623581954</v>
+        <v>1.283760190371393</v>
       </c>
       <c r="N7" t="n">
-        <v>1.624161506023638</v>
+        <v>1.207267232655584</v>
       </c>
       <c r="O7" t="n">
-        <v>1.600572106795038</v>
+        <v>1.198465991177769</v>
       </c>
       <c r="P7" t="n">
-        <v>1.559977051378325</v>
+        <v>1.21845740230329</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.540175940260056</v>
+        <v>1.247000909120446</v>
       </c>
       <c r="R7" t="n">
-        <v>1.522688733936578</v>
+        <v>1.264884495312409</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.005878016072274912</v>
+        <v>0.3707424438338888</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6852806496589756</v>
+        <v>0.7069235210674011</v>
       </c>
       <c r="C8" t="n">
-        <v>1.707709121692729</v>
+        <v>0.9757870281078138</v>
       </c>
       <c r="D8" t="n">
-        <v>2.88831721492936</v>
+        <v>1.188337238296828</v>
       </c>
       <c r="E8" t="n">
-        <v>2.767623942478496</v>
+        <v>2.05211858513981</v>
       </c>
       <c r="F8" t="n">
-        <v>2.966047076824905</v>
+        <v>2.122659222846991</v>
       </c>
       <c r="G8" t="n">
-        <v>2.127341954022043</v>
+        <v>2.209273681017133</v>
       </c>
       <c r="H8" t="n">
-        <v>2.281233850384425</v>
+        <v>2.066352463045146</v>
       </c>
       <c r="I8" t="n">
-        <v>1.814987420341731</v>
+        <v>1.75584762544104</v>
       </c>
       <c r="J8" t="n">
-        <v>1.702788080782125</v>
+        <v>1.565996481394698</v>
       </c>
       <c r="K8" t="n">
-        <v>1.495741857926718</v>
+        <v>1.406009446552929</v>
       </c>
       <c r="L8" t="n">
-        <v>1.641438359777496</v>
+        <v>1.27446576656565</v>
       </c>
       <c r="M8" t="n">
-        <v>1.648844311548886</v>
+        <v>1.267293663965362</v>
       </c>
       <c r="N8" t="n">
-        <v>1.63067766147984</v>
+        <v>1.216574635391467</v>
       </c>
       <c r="O8" t="n">
-        <v>1.59953453748055</v>
+        <v>1.213894237004924</v>
       </c>
       <c r="P8" t="n">
-        <v>1.549865589953273</v>
+        <v>1.239961640821743</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.530168510815363</v>
+        <v>1.264108513303466</v>
       </c>
       <c r="R8" t="n">
-        <v>1.515323492772303</v>
+        <v>1.278613605605301</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.007896522868499725</v>
+        <v>0.4612301545497855</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6827431984863764</v>
+        <v>0.6741578587291412</v>
       </c>
       <c r="C9" t="n">
-        <v>1.678067789774842</v>
+        <v>0.8553524274642381</v>
       </c>
       <c r="D9" t="n">
-        <v>2.801112447162808</v>
+        <v>1.144785844182403</v>
       </c>
       <c r="E9" t="n">
-        <v>2.727727556133826</v>
+        <v>1.752065230504687</v>
       </c>
       <c r="F9" t="n">
-        <v>2.979261801632777</v>
+        <v>1.882227077251245</v>
       </c>
       <c r="G9" t="n">
-        <v>2.155666851270604</v>
+        <v>2.240700074452763</v>
       </c>
       <c r="H9" t="n">
-        <v>2.264307860363919</v>
+        <v>1.952996589018401</v>
       </c>
       <c r="I9" t="n">
-        <v>1.796407217225291</v>
+        <v>1.757050751247452</v>
       </c>
       <c r="J9" t="n">
-        <v>1.72433607158985</v>
+        <v>1.581575670373326</v>
       </c>
       <c r="K9" t="n">
-        <v>1.486350386130828</v>
+        <v>1.414709363308954</v>
       </c>
       <c r="L9" t="n">
-        <v>1.630274727892538</v>
+        <v>1.296262737160476</v>
       </c>
       <c r="M9" t="n">
-        <v>1.647459762544687</v>
+        <v>1.241281150941194</v>
       </c>
       <c r="N9" t="n">
-        <v>1.631048172496801</v>
+        <v>1.232817827446904</v>
       </c>
       <c r="O9" t="n">
-        <v>1.592551615326303</v>
+        <v>1.221956966106054</v>
       </c>
       <c r="P9" t="n">
-        <v>1.5351964444981</v>
+        <v>1.242418553342275</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.515242967171427</v>
+        <v>1.262038550656351</v>
       </c>
       <c r="R9" t="n">
-        <v>1.503595480535878</v>
+        <v>1.273352068254372</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.01060818355139448</v>
+        <v>0.5738033478609053</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6794117554120129</v>
+        <v>0.6425395223291118</v>
       </c>
       <c r="C10" t="n">
-        <v>1.634589649597641</v>
+        <v>0.7277008111055865</v>
       </c>
       <c r="D10" t="n">
-        <v>2.693295871282166</v>
+        <v>1.08324992748554</v>
       </c>
       <c r="E10" t="n">
-        <v>2.682223191260612</v>
+        <v>1.529277313059362</v>
       </c>
       <c r="F10" t="n">
-        <v>2.990392120498459</v>
+        <v>1.882032015685485</v>
       </c>
       <c r="G10" t="n">
-        <v>2.182346235276537</v>
+        <v>2.259990904132687</v>
       </c>
       <c r="H10" t="n">
-        <v>2.234122349994617</v>
+        <v>1.969142748427805</v>
       </c>
       <c r="I10" t="n">
-        <v>1.777570675218598</v>
+        <v>1.749522650794946</v>
       </c>
       <c r="J10" t="n">
-        <v>1.745971528425862</v>
+        <v>1.576342364538444</v>
       </c>
       <c r="K10" t="n">
-        <v>1.494428953651021</v>
+        <v>1.420646181314003</v>
       </c>
       <c r="L10" t="n">
-        <v>1.612802388281809</v>
+        <v>1.30498895735583</v>
       </c>
       <c r="M10" t="n">
-        <v>1.639290047436793</v>
+        <v>1.269392837657998</v>
       </c>
       <c r="N10" t="n">
-        <v>1.624285152044424</v>
+        <v>1.2469101496431</v>
       </c>
       <c r="O10" t="n">
-        <v>1.579039880526794</v>
+        <v>1.221831229033579</v>
       </c>
       <c r="P10" t="n">
-        <v>1.515932586834172</v>
+        <v>1.225151358004142</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.513385745266462</v>
+        <v>1.240185770226092</v>
       </c>
       <c r="R10" t="n">
-        <v>1.522597085759018</v>
+        <v>1.248473479980733</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.01425102670302998</v>
+        <v>0.7138524633927497</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6750724385957115</v>
+        <v>0.6129024434653347</v>
       </c>
       <c r="C11" t="n">
-        <v>1.573685888016534</v>
+        <v>0.6538978740290342</v>
       </c>
       <c r="D11" t="n">
-        <v>2.561111060689592</v>
+        <v>1.003199965811181</v>
       </c>
       <c r="E11" t="n">
-        <v>2.628769228984412</v>
+        <v>1.452696456169148</v>
       </c>
       <c r="F11" t="n">
-        <v>2.996886943244776</v>
+        <v>1.90800142584082</v>
       </c>
       <c r="G11" t="n">
-        <v>2.20534024255213</v>
+        <v>2.265875902562741</v>
       </c>
       <c r="H11" t="n">
-        <v>2.189764056709101</v>
+        <v>1.957174450963632</v>
       </c>
       <c r="I11" t="n">
-        <v>1.764370732834754</v>
+        <v>1.718570514174971</v>
       </c>
       <c r="J11" t="n">
-        <v>1.786805412558994</v>
+        <v>1.553266106132795</v>
       </c>
       <c r="K11" t="n">
-        <v>1.536309307508362</v>
+        <v>1.425213392320913</v>
       </c>
       <c r="L11" t="n">
-        <v>1.588846489854263</v>
+        <v>1.310632634401007</v>
       </c>
       <c r="M11" t="n">
-        <v>1.622987738551814</v>
+        <v>1.281775821475259</v>
       </c>
       <c r="N11" t="n">
-        <v>1.608948904270082</v>
+        <v>1.240352009991035</v>
       </c>
       <c r="O11" t="n">
-        <v>1.558003093136675</v>
+        <v>1.209188641979119</v>
       </c>
       <c r="P11" t="n">
-        <v>1.541272336579834</v>
+        <v>1.211321287241245</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.556812524402177</v>
+        <v>1.240691670352237</v>
       </c>
       <c r="R11" t="n">
-        <v>1.56352186245963</v>
+        <v>1.265572230902107</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.01914481976169958</v>
+        <v>0.8880835941295776</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6694672911126558</v>
+        <v>0.5863363270114194</v>
       </c>
       <c r="C12" t="n">
-        <v>1.491748078876253</v>
+        <v>0.6398954653590745</v>
       </c>
       <c r="D12" t="n">
-        <v>2.401032936111297</v>
+        <v>0.8992482823287864</v>
       </c>
       <c r="E12" t="n">
-        <v>2.596086280799426</v>
+        <v>1.359606084558282</v>
       </c>
       <c r="F12" t="n">
-        <v>2.995593931482164</v>
+        <v>1.915274355067306</v>
       </c>
       <c r="G12" t="n">
-        <v>2.222633276220631</v>
+        <v>2.257200154453499</v>
       </c>
       <c r="H12" t="n">
-        <v>2.130494984471737</v>
+        <v>1.916979041575142</v>
       </c>
       <c r="I12" t="n">
-        <v>1.762643034112494</v>
+        <v>1.663638210876804</v>
       </c>
       <c r="J12" t="n">
-        <v>1.825664083779874</v>
+        <v>1.527946855238616</v>
       </c>
       <c r="K12" t="n">
-        <v>1.586742578854114</v>
+        <v>1.407754776381816</v>
       </c>
       <c r="L12" t="n">
-        <v>1.557952682985113</v>
+        <v>1.318889909595039</v>
       </c>
       <c r="M12" t="n">
-        <v>1.596807646548237</v>
+        <v>1.299342996509572</v>
       </c>
       <c r="N12" t="n">
-        <v>1.583081966349924</v>
+        <v>1.24421633460059</v>
       </c>
       <c r="O12" t="n">
-        <v>1.568965188743335</v>
+        <v>1.226573814870918</v>
       </c>
       <c r="P12" t="n">
-        <v>1.575881903209423</v>
+        <v>1.240421355412728</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.590234050434626</v>
+        <v>1.257390219957728</v>
       </c>
       <c r="R12" t="n">
-        <v>1.594290113655578</v>
+        <v>1.28033304052957</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.02571913809059344</v>
+        <v>1.104839600067588</v>
       </c>
       <c r="B13" t="n">
-        <v>0.6623091985419497</v>
+        <v>0.5641037151588262</v>
       </c>
       <c r="C13" t="n">
-        <v>1.385487088111278</v>
+        <v>0.6286889698727361</v>
       </c>
       <c r="D13" t="n">
-        <v>2.209993068133039</v>
+        <v>0.8697725394200128</v>
       </c>
       <c r="E13" t="n">
-        <v>2.556855198482701</v>
+        <v>1.24920093464041</v>
       </c>
       <c r="F13" t="n">
-        <v>2.980679058127335</v>
+        <v>1.902490218469324</v>
       </c>
       <c r="G13" t="n">
-        <v>2.232156886460375</v>
+        <v>2.207535906200504</v>
       </c>
       <c r="H13" t="n">
-        <v>2.083335431299749</v>
+        <v>1.849007290340861</v>
       </c>
       <c r="I13" t="n">
-        <v>1.75750363558898</v>
+        <v>1.606190051236497</v>
       </c>
       <c r="J13" t="n">
-        <v>1.854544356543326</v>
+        <v>1.526843510966136</v>
       </c>
       <c r="K13" t="n">
-        <v>1.627757534844874</v>
+        <v>1.394891652580279</v>
       </c>
       <c r="L13" t="n">
-        <v>1.550725406850607</v>
+        <v>1.348751026178271</v>
       </c>
       <c r="M13" t="n">
-        <v>1.556867335327786</v>
+        <v>1.329977714557359</v>
       </c>
       <c r="N13" t="n">
-        <v>1.566037926215166</v>
+        <v>1.277046346740933</v>
       </c>
       <c r="O13" t="n">
-        <v>1.572677495857805</v>
+        <v>1.251750590074114</v>
       </c>
       <c r="P13" t="n">
-        <v>1.5684703418324</v>
+        <v>1.261192690135161</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.571423423910623</v>
+        <v>1.27440212233546</v>
       </c>
       <c r="R13" t="n">
-        <v>1.568335191084607</v>
+        <v>1.294132962839453</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.03455107294592218</v>
+        <v>1.374499596599242</v>
       </c>
       <c r="B14" t="n">
-        <v>0.6532922412478379</v>
+        <v>0.5474684463078364</v>
       </c>
       <c r="C14" t="n">
-        <v>1.254189078645948</v>
+        <v>0.6203035192652381</v>
       </c>
       <c r="D14" t="n">
-        <v>1.985524427780957</v>
+        <v>0.8456995832693768</v>
       </c>
       <c r="E14" t="n">
-        <v>2.499364006682315</v>
+        <v>1.122127874471816</v>
       </c>
       <c r="F14" t="n">
-        <v>2.947111795251171</v>
+        <v>1.868479355607811</v>
       </c>
       <c r="G14" t="n">
-        <v>2.231720991179159</v>
+        <v>2.118882534897368</v>
       </c>
       <c r="H14" t="n">
-        <v>2.047271278253446</v>
+        <v>1.754300749996815</v>
       </c>
       <c r="I14" t="n">
-        <v>1.746435921098354</v>
+        <v>1.587332491926374</v>
       </c>
       <c r="J14" t="n">
-        <v>1.834528923295452</v>
+        <v>1.5362474662948</v>
       </c>
       <c r="K14" t="n">
-        <v>1.622397311927074</v>
+        <v>1.424497140254504</v>
       </c>
       <c r="L14" t="n">
-        <v>1.532272597241757</v>
+        <v>1.365510089622552</v>
       </c>
       <c r="M14" t="n">
-        <v>1.511982300049339</v>
+        <v>1.338952094961337</v>
       </c>
       <c r="N14" t="n">
-        <v>1.519388241994789</v>
+        <v>1.289026031587522</v>
       </c>
       <c r="O14" t="n">
-        <v>1.525910138568968</v>
+        <v>1.259495731241599</v>
       </c>
       <c r="P14" t="n">
-        <v>1.523443394642742</v>
+        <v>1.264321465524143</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.526433470953279</v>
+        <v>1.273564330689421</v>
       </c>
       <c r="R14" t="n">
-        <v>1.521488660861674</v>
+        <v>1.289707232085352</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.04641588833612777</v>
+        <v>1.709975946676696</v>
       </c>
       <c r="B15" t="n">
-        <v>0.6421172316111639</v>
+        <v>0.5398758018461325</v>
       </c>
       <c r="C15" t="n">
-        <v>1.206633395829892</v>
+        <v>0.6147464939889941</v>
       </c>
       <c r="D15" t="n">
-        <v>1.725945531993205</v>
+        <v>0.8195738202326646</v>
       </c>
       <c r="E15" t="n">
-        <v>2.422836988860334</v>
+        <v>0.9865534516257667</v>
       </c>
       <c r="F15" t="n">
-        <v>2.889991693087042</v>
+        <v>1.783319468333747</v>
       </c>
       <c r="G15" t="n">
-        <v>2.192133648410938</v>
+        <v>2.017411352077881</v>
       </c>
       <c r="H15" t="n">
-        <v>1.954139073443558</v>
+        <v>1.65645618775807</v>
       </c>
       <c r="I15" t="n">
-        <v>1.725968992515734</v>
+        <v>1.558003930563377</v>
       </c>
       <c r="J15" t="n">
-        <v>1.778515842344669</v>
+        <v>1.526657123250654</v>
       </c>
       <c r="K15" t="n">
-        <v>1.583750454672446</v>
+        <v>1.464656113598734</v>
       </c>
       <c r="L15" t="n">
-        <v>1.489294046286073</v>
+        <v>1.403633689677934</v>
       </c>
       <c r="M15" t="n">
-        <v>1.458559965314468</v>
+        <v>1.381434957734616</v>
       </c>
       <c r="N15" t="n">
-        <v>1.459721108977295</v>
+        <v>1.334255308173018</v>
       </c>
       <c r="O15" t="n">
-        <v>1.46494033863979</v>
+        <v>1.287168477421415</v>
       </c>
       <c r="P15" t="n">
-        <v>1.463421125489342</v>
+        <v>1.27478337004988</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.465952535356177</v>
+        <v>1.277752060823033</v>
       </c>
       <c r="R15" t="n">
-        <v>1.459532785066383</v>
+        <v>1.297312240589245</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.06235507341273912</v>
+        <v>2.12733255466019</v>
       </c>
       <c r="B16" t="n">
-        <v>0.6279874910775751</v>
+        <v>0.558687702763609</v>
       </c>
       <c r="C16" t="n">
-        <v>1.127573302416302</v>
+        <v>0.611946469993168</v>
       </c>
       <c r="D16" t="n">
-        <v>1.475090050759167</v>
+        <v>0.7934615393115265</v>
       </c>
       <c r="E16" t="n">
-        <v>2.326703592806351</v>
+        <v>0.8833210226226786</v>
       </c>
       <c r="F16" t="n">
-        <v>2.74562386668508</v>
+        <v>1.663858548378745</v>
       </c>
       <c r="G16" t="n">
-        <v>2.109702534764569</v>
+        <v>1.902440374953978</v>
       </c>
       <c r="H16" t="n">
-        <v>1.787290593776966</v>
+        <v>1.608604874433645</v>
       </c>
       <c r="I16" t="n">
-        <v>1.64519435656293</v>
+        <v>1.545276775437447</v>
       </c>
       <c r="J16" t="n">
-        <v>1.709252597201016</v>
+        <v>1.553403109796021</v>
       </c>
       <c r="K16" t="n">
-        <v>1.531757469386132</v>
+        <v>1.491848451407574</v>
       </c>
       <c r="L16" t="n">
-        <v>1.432476182842028</v>
+        <v>1.431706216871707</v>
       </c>
       <c r="M16" t="n">
-        <v>1.390904439150175</v>
+        <v>1.411988055174287</v>
       </c>
       <c r="N16" t="n">
-        <v>1.384687955887528</v>
+        <v>1.368710045392602</v>
       </c>
       <c r="O16" t="n">
-        <v>1.387328947646518</v>
+        <v>1.323115000954781</v>
       </c>
       <c r="P16" t="n">
-        <v>1.385812749903943</v>
+        <v>1.313115234436891</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.387314941771849</v>
+        <v>1.319032389427746</v>
       </c>
       <c r="R16" t="n">
-        <v>1.37972844143468</v>
+        <v>1.326815714304674</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.08376776400682916</v>
+        <v>2.646554068150696</v>
       </c>
       <c r="B17" t="n">
-        <v>0.6091827949303438</v>
+        <v>0.5700677567761342</v>
       </c>
       <c r="C17" t="n">
-        <v>1.020279714515212</v>
+        <v>0.6117277244346779</v>
       </c>
       <c r="D17" t="n">
-        <v>1.296266347848598</v>
+        <v>0.7537504244704878</v>
       </c>
       <c r="E17" t="n">
-        <v>2.210464721344918</v>
+        <v>0.8801263292265694</v>
       </c>
       <c r="F17" t="n">
-        <v>2.579302014939824</v>
+        <v>1.556020406993353</v>
       </c>
       <c r="G17" t="n">
-        <v>2.013832921383506</v>
+        <v>1.790332745277128</v>
       </c>
       <c r="H17" t="n">
-        <v>1.627333755397417</v>
+        <v>1.555243564588608</v>
       </c>
       <c r="I17" t="n">
-        <v>1.546437181919534</v>
+        <v>1.548757305048425</v>
       </c>
       <c r="J17" t="n">
-        <v>1.623824819890437</v>
+        <v>1.571515394551728</v>
       </c>
       <c r="K17" t="n">
-        <v>1.464275931931925</v>
+        <v>1.502970484876297</v>
       </c>
       <c r="L17" t="n">
-        <v>1.359708598921821</v>
+        <v>1.436859908133851</v>
       </c>
       <c r="M17" t="n">
-        <v>1.30720009399002</v>
+        <v>1.416933096284825</v>
       </c>
       <c r="N17" t="n">
-        <v>1.292683783058779</v>
+        <v>1.37774330201389</v>
       </c>
       <c r="O17" t="n">
-        <v>1.29145968048906</v>
+        <v>1.344980062962306</v>
       </c>
       <c r="P17" t="n">
-        <v>1.288894663565466</v>
+        <v>1.340682489283512</v>
       </c>
       <c r="Q17" t="n">
-        <v>1.288739577481286</v>
+        <v>1.344098550132737</v>
       </c>
       <c r="R17" t="n">
-        <v>1.280195079718836</v>
+        <v>1.349385787581079</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1125335582600765</v>
+        <v>3.29250282016383</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5873804952299576</v>
+        <v>0.5781698651774043</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9083352872423262</v>
+        <v>0.6190676536884918</v>
       </c>
       <c r="D18" t="n">
-        <v>1.263073873897171</v>
+        <v>0.735298206119671</v>
       </c>
       <c r="E18" t="n">
-        <v>2.073632432259972</v>
+        <v>0.8592860498600493</v>
       </c>
       <c r="F18" t="n">
-        <v>2.391397868582826</v>
+        <v>1.503055693050448</v>
       </c>
       <c r="G18" t="n">
-        <v>1.903538368412157</v>
+        <v>1.666359212152981</v>
       </c>
       <c r="H18" t="n">
-        <v>1.625818651229139</v>
+        <v>1.487186434463464</v>
       </c>
       <c r="I18" t="n">
-        <v>1.433466040885883</v>
+        <v>1.558982511054388</v>
       </c>
       <c r="J18" t="n">
-        <v>1.519550012052634</v>
+        <v>1.608172806475934</v>
       </c>
       <c r="K18" t="n">
-        <v>1.379391344851015</v>
+        <v>1.53002596261886</v>
       </c>
       <c r="L18" t="n">
-        <v>1.27944249167003</v>
+        <v>1.463111648592055</v>
       </c>
       <c r="M18" t="n">
-        <v>1.216637951617226</v>
+        <v>1.432705573617592</v>
       </c>
       <c r="N18" t="n">
-        <v>1.190761555554248</v>
+        <v>1.394107897484623</v>
       </c>
       <c r="O18" t="n">
-        <v>1.187825002459584</v>
+        <v>1.361997086518806</v>
       </c>
       <c r="P18" t="n">
-        <v>1.19064515687612</v>
+        <v>1.355935381480177</v>
       </c>
       <c r="Q18" t="n">
-        <v>1.193135716758299</v>
+        <v>1.361140674676863</v>
       </c>
       <c r="R18" t="n">
-        <v>1.189442446085842</v>
+        <v>1.370198776587459</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1511775070615662</v>
+        <v>4.096109333735141</v>
       </c>
       <c r="B19" t="n">
-        <v>0.562689224586151</v>
+        <v>0.5885258352124072</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8172658544856909</v>
+        <v>0.6283978600229053</v>
       </c>
       <c r="D19" t="n">
-        <v>1.202653339338999</v>
+        <v>0.7320374638921172</v>
       </c>
       <c r="E19" t="n">
-        <v>1.965923176476822</v>
+        <v>0.8555260289766001</v>
       </c>
       <c r="F19" t="n">
-        <v>2.183383782964184</v>
+        <v>1.417269466741537</v>
       </c>
       <c r="G19" t="n">
-        <v>1.778923924663338</v>
+        <v>1.516849993167414</v>
       </c>
       <c r="H19" t="n">
-        <v>1.680061625952451</v>
+        <v>1.485586461743118</v>
       </c>
       <c r="I19" t="n">
-        <v>1.389053772460471</v>
+        <v>1.583248682751186</v>
       </c>
       <c r="J19" t="n">
-        <v>1.407495829694825</v>
+        <v>1.619277062485059</v>
       </c>
       <c r="K19" t="n">
-        <v>1.322225928470938</v>
+        <v>1.533550345503808</v>
       </c>
       <c r="L19" t="n">
-        <v>1.239219747622664</v>
+        <v>1.466983755237365</v>
       </c>
       <c r="M19" t="n">
-        <v>1.172306096276725</v>
+        <v>1.443189073461332</v>
       </c>
       <c r="N19" t="n">
-        <v>1.139361048009241</v>
+        <v>1.415998107962315</v>
       </c>
       <c r="O19" t="n">
-        <v>1.130553741011169</v>
+        <v>1.386296556958543</v>
       </c>
       <c r="P19" t="n">
-        <v>1.130225881354878</v>
+        <v>1.379876992331355</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.130087676997644</v>
+        <v>1.38265953108488</v>
       </c>
       <c r="R19" t="n">
-        <v>1.124915555753674</v>
+        <v>1.388670055719298</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.2030917620904735</v>
+        <v>5.09585339491897</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5353728340183243</v>
+        <v>0.6010476767489764</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7413525346430925</v>
+        <v>0.6379714724570519</v>
       </c>
       <c r="D20" t="n">
-        <v>1.122924742686539</v>
+        <v>0.7297278476833288</v>
       </c>
       <c r="E20" t="n">
-        <v>1.828863799708498</v>
+        <v>0.8397535216241669</v>
       </c>
       <c r="F20" t="n">
-        <v>1.957678615135108</v>
+        <v>1.298980704247115</v>
       </c>
       <c r="G20" t="n">
-        <v>1.826072270307782</v>
+        <v>1.404263047065973</v>
       </c>
       <c r="H20" t="n">
-        <v>1.732138825802584</v>
+        <v>1.468649204466867</v>
       </c>
       <c r="I20" t="n">
-        <v>1.420391321506225</v>
+        <v>1.597144101106145</v>
       </c>
       <c r="J20" t="n">
-        <v>1.291084277514666</v>
+        <v>1.605565850803067</v>
       </c>
       <c r="K20" t="n">
-        <v>1.264915876544173</v>
+        <v>1.529202059687508</v>
       </c>
       <c r="L20" t="n">
-        <v>1.182661007329773</v>
+        <v>1.475495972507496</v>
       </c>
       <c r="M20" t="n">
-        <v>1.112794550809379</v>
+        <v>1.440918683275737</v>
       </c>
       <c r="N20" t="n">
-        <v>1.073599738798701</v>
+        <v>1.415885272560535</v>
       </c>
       <c r="O20" t="n">
-        <v>1.058749325706038</v>
+        <v>1.388669205424888</v>
       </c>
       <c r="P20" t="n">
-        <v>1.054458378491506</v>
+        <v>1.382095716746994</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.051243126406144</v>
+        <v>1.387264789568802</v>
       </c>
       <c r="R20" t="n">
-        <v>1.044527837933746</v>
+        <v>1.39559576420596</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.2728333376486767</v>
+        <v>6.339606613680861</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5058500726568148</v>
+        <v>0.616243230984456</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6640813508070266</v>
+        <v>0.6478004137292941</v>
       </c>
       <c r="D21" t="n">
-        <v>1.099322507580134</v>
+        <v>0.7284605470874026</v>
       </c>
       <c r="E21" t="n">
-        <v>1.667025646766613</v>
+        <v>0.8162477863676854</v>
       </c>
       <c r="F21" t="n">
-        <v>1.71735074859468</v>
+        <v>1.177004829364878</v>
       </c>
       <c r="G21" t="n">
-        <v>1.876218300458364</v>
+        <v>1.338508238650408</v>
       </c>
       <c r="H21" t="n">
-        <v>1.773885778143179</v>
+        <v>1.440172023027811</v>
       </c>
       <c r="I21" t="n">
-        <v>1.461935559918561</v>
+        <v>1.58702735913072</v>
       </c>
       <c r="J21" t="n">
-        <v>1.174988481475346</v>
+        <v>1.604243629169648</v>
       </c>
       <c r="K21" t="n">
-        <v>1.189702079187085</v>
+        <v>1.540749546640046</v>
       </c>
       <c r="L21" t="n">
-        <v>1.109844715356376</v>
+        <v>1.487517665339947</v>
       </c>
       <c r="M21" t="n">
-        <v>1.038737486967558</v>
+        <v>1.453616962425742</v>
       </c>
       <c r="N21" t="n">
-        <v>0.9945344246783955</v>
+        <v>1.427897473538726</v>
       </c>
       <c r="O21" t="n">
-        <v>0.9739039582553671</v>
+        <v>1.40185420258834</v>
       </c>
       <c r="P21" t="n">
-        <v>0.9652212448715064</v>
+        <v>1.394933781677841</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.9588121389559291</v>
+        <v>1.395837134903557</v>
       </c>
       <c r="R21" t="n">
-        <v>0.9572074957712293</v>
+        <v>1.404761454758362</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.3665241237079626</v>
+        <v>7.886924701621083</v>
       </c>
       <c r="B22" t="n">
-        <v>0.4747338405652452</v>
+        <v>0.6367462553167853</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5889077743611248</v>
+        <v>0.6654734634230701</v>
       </c>
       <c r="D22" t="n">
-        <v>1.050837574372316</v>
+        <v>0.7338140462494046</v>
       </c>
       <c r="E22" t="n">
-        <v>1.478255061520342</v>
+        <v>0.7949933550396473</v>
       </c>
       <c r="F22" t="n">
-        <v>1.505661166688557</v>
+        <v>1.06444325387071</v>
       </c>
       <c r="G22" t="n">
-        <v>1.896459727070639</v>
+        <v>1.276354119299158</v>
       </c>
       <c r="H22" t="n">
-        <v>1.797087387011316</v>
+        <v>1.43960940772326</v>
       </c>
       <c r="I22" t="n">
-        <v>1.481394736418967</v>
+        <v>1.554362440103585</v>
       </c>
       <c r="J22" t="n">
-        <v>1.167163197735204</v>
+        <v>1.599195722082072</v>
       </c>
       <c r="K22" t="n">
-        <v>1.096835536692827</v>
+        <v>1.531167114542503</v>
       </c>
       <c r="L22" t="n">
-        <v>1.021826103256305</v>
+        <v>1.488213046835177</v>
       </c>
       <c r="M22" t="n">
-        <v>0.9518559096059932</v>
+        <v>1.453585219761068</v>
       </c>
       <c r="N22" t="n">
-        <v>0.9431832259319548</v>
+        <v>1.427590775033584</v>
       </c>
       <c r="O22" t="n">
-        <v>0.9439278147964056</v>
+        <v>1.402960285727399</v>
       </c>
       <c r="P22" t="n">
-        <v>0.9540367931929243</v>
+        <v>1.399354173068766</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.9621913821199689</v>
+        <v>1.403199353942246</v>
       </c>
       <c r="R22" t="n">
-        <v>0.9675076038347056</v>
+        <v>1.410291631385475</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.4923882631706736</v>
+        <v>9.811899229647093</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4429308014239784</v>
+        <v>0.6596912834327305</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5196741310610729</v>
+        <v>0.6903949665304857</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9723652712875881</v>
+        <v>0.7450392753938296</v>
       </c>
       <c r="E23" t="n">
-        <v>1.260377031287007</v>
+        <v>0.7776056924221779</v>
       </c>
       <c r="F23" t="n">
-        <v>1.54417588746309</v>
+        <v>0.9565900150303335</v>
       </c>
       <c r="G23" t="n">
-        <v>1.91050992026191</v>
+        <v>1.230244549561914</v>
       </c>
       <c r="H23" t="n">
-        <v>1.79420385892299</v>
+        <v>1.416516560544935</v>
       </c>
       <c r="I23" t="n">
-        <v>1.472707215701778</v>
+        <v>1.545279185354805</v>
       </c>
       <c r="J23" t="n">
-        <v>1.178775110234252</v>
+        <v>1.573124798476239</v>
       </c>
       <c r="K23" t="n">
-        <v>1.012414072521156</v>
+        <v>1.530044068654824</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9648273473011874</v>
+        <v>1.507732437641101</v>
       </c>
       <c r="M23" t="n">
-        <v>0.9427794722626571</v>
+        <v>1.472757100857774</v>
       </c>
       <c r="N23" t="n">
-        <v>0.9458568294654934</v>
+        <v>1.439285831158521</v>
       </c>
       <c r="O23" t="n">
-        <v>0.9426829031185531</v>
+        <v>1.415034644281919</v>
       </c>
       <c r="P23" t="n">
-        <v>0.9468477216060317</v>
+        <v>1.417254726568804</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.9520256615200833</v>
+        <v>1.414089408340774</v>
       </c>
       <c r="R23" t="n">
-        <v>0.9539074268852562</v>
+        <v>1.417319582182156</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.6614740641230146</v>
+        <v>12.20670541877509</v>
       </c>
       <c r="B24" t="n">
-        <v>0.411807614632429</v>
+        <v>0.6845200759824653</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4605122992773123</v>
+        <v>0.7159327226430585</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8646713639392213</v>
+        <v>0.7625560691670743</v>
       </c>
       <c r="E24" t="n">
-        <v>1.157503142750255</v>
+        <v>0.7851013390262824</v>
       </c>
       <c r="F24" t="n">
-        <v>1.563490141613301</v>
+        <v>0.921750663420298</v>
       </c>
       <c r="G24" t="n">
-        <v>1.92596763646758</v>
+        <v>1.183034317676104</v>
       </c>
       <c r="H24" t="n">
-        <v>1.758900058096985</v>
+        <v>1.37211941316352</v>
       </c>
       <c r="I24" t="n">
-        <v>1.431129260758631</v>
+        <v>1.520592550932615</v>
       </c>
       <c r="J24" t="n">
-        <v>1.159169578505931</v>
+        <v>1.557182173316758</v>
       </c>
       <c r="K24" t="n">
-        <v>1.008331246189081</v>
+        <v>1.533214367636024</v>
       </c>
       <c r="L24" t="n">
-        <v>0.958072629313273</v>
+        <v>1.507137067177687</v>
       </c>
       <c r="M24" t="n">
-        <v>0.9255948392907902</v>
+        <v>1.47436471218374</v>
       </c>
       <c r="N24" t="n">
-        <v>0.9202042617082613</v>
+        <v>1.44213727522003</v>
       </c>
       <c r="O24" t="n">
-        <v>0.9123026751283314</v>
+        <v>1.43400259408501</v>
       </c>
       <c r="P24" t="n">
-        <v>0.9106712499649949</v>
+        <v>1.432841870449608</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.9226416932521599</v>
+        <v>1.426245701986494</v>
       </c>
       <c r="R24" t="n">
-        <v>0.9367141421466978</v>
+        <v>1.425462682907907</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.8886238162743398</v>
+        <v>15.18601584599768</v>
       </c>
       <c r="B25" t="n">
-        <v>0.3833643077043861</v>
+        <v>0.7107518694982766</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4155184175461208</v>
+        <v>0.7418889056904394</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7280196566135586</v>
+        <v>0.7824067279183173</v>
       </c>
       <c r="E25" t="n">
-        <v>1.078191836228708</v>
+        <v>0.7949850717722794</v>
       </c>
       <c r="F25" t="n">
-        <v>1.557938379461655</v>
+        <v>0.921825057928384</v>
       </c>
       <c r="G25" t="n">
-        <v>1.915008902824143</v>
+        <v>1.156881511489226</v>
       </c>
       <c r="H25" t="n">
-        <v>1.698650246002502</v>
+        <v>1.326934891612254</v>
       </c>
       <c r="I25" t="n">
-        <v>1.373514104461262</v>
+        <v>1.477205319220624</v>
       </c>
       <c r="J25" t="n">
-        <v>1.147999540780959</v>
+        <v>1.547660463095287</v>
       </c>
       <c r="K25" t="n">
-        <v>0.9952412102831132</v>
+        <v>1.515885018348927</v>
       </c>
       <c r="L25" t="n">
-        <v>0.9458116842530411</v>
+        <v>1.52173850884783</v>
       </c>
       <c r="M25" t="n">
-        <v>0.9155923110653117</v>
+        <v>1.494854046881497</v>
       </c>
       <c r="N25" t="n">
-        <v>0.9177993313094919</v>
+        <v>1.458562226599124</v>
       </c>
       <c r="O25" t="n">
-        <v>0.9217476541294835</v>
+        <v>1.435059531679999</v>
       </c>
       <c r="P25" t="n">
-        <v>0.9260449700765603</v>
+        <v>1.427608017041678</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.9348234220495786</v>
+        <v>1.417994878346536</v>
       </c>
       <c r="R25" t="n">
-        <v>0.9454133648480729</v>
+        <v>1.413545648409175</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.193776641714436</v>
+        <v>18.89249141051478</v>
       </c>
       <c r="B26" t="n">
-        <v>0.3602617132741491</v>
+        <v>0.7381025386381806</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4078961671419372</v>
+        <v>0.7681092771959888</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5724490363396998</v>
+        <v>0.797123688028275</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9667021847121495</v>
+        <v>0.8070356159852611</v>
       </c>
       <c r="F26" t="n">
-        <v>1.522009496128245</v>
+        <v>0.9129842672527718</v>
       </c>
       <c r="G26" t="n">
-        <v>1.829840541763049</v>
+        <v>1.135611675047124</v>
       </c>
       <c r="H26" t="n">
-        <v>1.610572179061693</v>
+        <v>1.304068919930042</v>
       </c>
       <c r="I26" t="n">
-        <v>1.347525240186666</v>
+        <v>1.448929913431626</v>
       </c>
       <c r="J26" t="n">
-        <v>1.152718199694026</v>
+        <v>1.518483719423855</v>
       </c>
       <c r="K26" t="n">
-        <v>1.013384635442042</v>
+        <v>1.516010242183045</v>
       </c>
       <c r="L26" t="n">
-        <v>0.9636840986302655</v>
+        <v>1.525914142367004</v>
       </c>
       <c r="M26" t="n">
-        <v>0.9265599231097236</v>
+        <v>1.494403434899745</v>
       </c>
       <c r="N26" t="n">
-        <v>0.9213788605047827</v>
+        <v>1.456217007315608</v>
       </c>
       <c r="O26" t="n">
-        <v>0.9197612444603209</v>
+        <v>1.433334079328557</v>
       </c>
       <c r="P26" t="n">
-        <v>0.9186810911435503</v>
+        <v>1.431382630475118</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.9236147912376443</v>
+        <v>1.422064703261476</v>
       </c>
       <c r="R26" t="n">
-        <v>0.9302784359452958</v>
+        <v>1.417388151589226</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1.603718743751329</v>
+        <v>23.50361248901527</v>
       </c>
       <c r="B27" t="n">
-        <v>0.3454677823890407</v>
+        <v>0.7663153962195259</v>
       </c>
       <c r="C27" t="n">
-        <v>0.4075426143241028</v>
+        <v>0.7944888037010905</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5431158605474632</v>
+        <v>0.8124341720152646</v>
       </c>
       <c r="E27" t="n">
-        <v>0.824286747552758</v>
+        <v>0.820810135464376</v>
       </c>
       <c r="F27" t="n">
-        <v>1.434883971716105</v>
+        <v>0.8969628037990784</v>
       </c>
       <c r="G27" t="n">
-        <v>1.710491014023129</v>
+        <v>1.102219979970656</v>
       </c>
       <c r="H27" t="n">
-        <v>1.516545109767284</v>
+        <v>1.267082644941159</v>
       </c>
       <c r="I27" t="n">
-        <v>1.3093267701997</v>
+        <v>1.423036747259841</v>
       </c>
       <c r="J27" t="n">
-        <v>1.135561989321261</v>
+        <v>1.501755168503612</v>
       </c>
       <c r="K27" t="n">
-        <v>1.012280287275241</v>
+        <v>1.50973073186477</v>
       </c>
       <c r="L27" t="n">
-        <v>0.9578043296169276</v>
+        <v>1.508675173890197</v>
       </c>
       <c r="M27" t="n">
-        <v>0.919061353497848</v>
+        <v>1.47554915795236</v>
       </c>
       <c r="N27" t="n">
-        <v>0.9016092721491755</v>
+        <v>1.451309689236889</v>
       </c>
       <c r="O27" t="n">
-        <v>0.8942506307930229</v>
+        <v>1.434488389485495</v>
       </c>
       <c r="P27" t="n">
-        <v>0.9043029391866957</v>
+        <v>1.428896442921088</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.9226676862858975</v>
+        <v>1.417103278436492</v>
       </c>
       <c r="R27" t="n">
-        <v>0.9290135152518284</v>
+        <v>1.409277153794802</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2.154434690031882</v>
+        <v>29.24017738212864</v>
       </c>
       <c r="B28" t="n">
-        <v>0.3556845960837771</v>
+        <v>0.795260886729663</v>
       </c>
       <c r="C28" t="n">
-        <v>0.408151466027002</v>
+        <v>0.8209722055387985</v>
       </c>
       <c r="D28" t="n">
-        <v>0.540674711242401</v>
+        <v>0.829432400990159</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6734570688959627</v>
+        <v>0.8360615028091541</v>
       </c>
       <c r="F28" t="n">
-        <v>1.283882083463149</v>
+        <v>0.8902077371189296</v>
       </c>
       <c r="G28" t="n">
-        <v>1.565783681429796</v>
+        <v>1.059369720843881</v>
       </c>
       <c r="H28" t="n">
-        <v>1.436199652125936</v>
+        <v>1.218991097298709</v>
       </c>
       <c r="I28" t="n">
-        <v>1.243243951297323</v>
+        <v>1.380657576312693</v>
       </c>
       <c r="J28" t="n">
-        <v>1.106580634836474</v>
+        <v>1.48822714523181</v>
       </c>
       <c r="K28" t="n">
-        <v>1.0248315038262</v>
+        <v>1.483518483063517</v>
       </c>
       <c r="L28" t="n">
-        <v>0.9780724990357471</v>
+        <v>1.501316973338546</v>
       </c>
       <c r="M28" t="n">
-        <v>0.9440086394474455</v>
+        <v>1.481109264758903</v>
       </c>
       <c r="N28" t="n">
-        <v>0.9224281618489405</v>
+        <v>1.453585782137143</v>
       </c>
       <c r="O28" t="n">
-        <v>0.9190657518791955</v>
+        <v>1.434189433585101</v>
       </c>
       <c r="P28" t="n">
-        <v>0.9174342083404764</v>
+        <v>1.414980082928444</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.9238103983257671</v>
+        <v>1.400488497365283</v>
       </c>
       <c r="R28" t="n">
-        <v>0.9310466262111614</v>
+        <v>1.394133892936341</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2.894266124716749</v>
+        <v>36.37687499051213</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3738442803572289</v>
+        <v>0.8247909974909531</v>
       </c>
       <c r="C29" t="n">
-        <v>0.4114224367800244</v>
+        <v>0.8475614264678747</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5296103689350711</v>
+        <v>0.848216408132811</v>
       </c>
       <c r="E29" t="n">
-        <v>0.639189752002165</v>
+        <v>0.8533062652235718</v>
       </c>
       <c r="F29" t="n">
-        <v>1.157195189110174</v>
+        <v>0.891585878853156</v>
       </c>
       <c r="G29" t="n">
-        <v>1.388049129167432</v>
+        <v>1.045992576301173</v>
       </c>
       <c r="H29" t="n">
-        <v>1.324359512361301</v>
+        <v>1.201201233997181</v>
       </c>
       <c r="I29" t="n">
-        <v>1.239367764405741</v>
+        <v>1.36460156982855</v>
       </c>
       <c r="J29" t="n">
-        <v>1.153337770416984</v>
+        <v>1.455632826439565</v>
       </c>
       <c r="K29" t="n">
-        <v>1.072080532703388</v>
+        <v>1.473247688078292</v>
       </c>
       <c r="L29" t="n">
-        <v>1.018300635779948</v>
+        <v>1.492342257305871</v>
       </c>
       <c r="M29" t="n">
-        <v>0.9806134708482409</v>
+        <v>1.468080302880831</v>
       </c>
       <c r="N29" t="n">
-        <v>0.9522048370305369</v>
+        <v>1.438141182123688</v>
       </c>
       <c r="O29" t="n">
-        <v>0.938105637775239</v>
+        <v>1.41689412137518</v>
       </c>
       <c r="P29" t="n">
-        <v>0.9331614765439098</v>
+        <v>1.401030647454684</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.9378958081617039</v>
+        <v>1.385736582067209</v>
       </c>
       <c r="R29" t="n">
-        <v>0.939292099146865</v>
+        <v>1.37690684295433</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3.888155180308085</v>
+        <v>45.2554379811705</v>
       </c>
       <c r="B30" t="n">
-        <v>0.3961906510978964</v>
+        <v>0.8546912245847453</v>
       </c>
       <c r="C30" t="n">
-        <v>0.4172827337468081</v>
+        <v>0.8743148334507822</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5092103108519688</v>
+        <v>0.8687678526109698</v>
       </c>
       <c r="E30" t="n">
-        <v>0.6187907506770359</v>
+        <v>0.8723722405586295</v>
       </c>
       <c r="F30" t="n">
-        <v>1.082856879568911</v>
+        <v>0.8907526217215125</v>
       </c>
       <c r="G30" t="n">
-        <v>1.189087229203833</v>
+        <v>1.028699965672837</v>
       </c>
       <c r="H30" t="n">
-        <v>1.230012394639936</v>
+        <v>1.171704147036456</v>
       </c>
       <c r="I30" t="n">
-        <v>1.219791834214635</v>
+        <v>1.340271193473707</v>
       </c>
       <c r="J30" t="n">
-        <v>1.169270962043614</v>
+        <v>1.435350776049678</v>
       </c>
       <c r="K30" t="n">
-        <v>1.086339482367875</v>
+        <v>1.45694802617511</v>
       </c>
       <c r="L30" t="n">
-        <v>1.0355500856858</v>
+        <v>1.465445462227573</v>
       </c>
       <c r="M30" t="n">
-        <v>1.002286263575929</v>
+        <v>1.438091665967313</v>
       </c>
       <c r="N30" t="n">
-        <v>0.9768305893551965</v>
+        <v>1.418443061530199</v>
       </c>
       <c r="O30" t="n">
-        <v>0.9655045827375062</v>
+        <v>1.408791497578475</v>
       </c>
       <c r="P30" t="n">
-        <v>0.9668642356922602</v>
+        <v>1.394209075048498</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.966772742770706</v>
+        <v>1.379009158580765</v>
       </c>
       <c r="R30" t="n">
-        <v>0.9684138029071532</v>
+        <v>1.369884000355497</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5.223345074266838</v>
+        <v>56.30100626845341</v>
       </c>
       <c r="B31" t="n">
-        <v>0.415022046735701</v>
+        <v>0.884933776953181</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4281995442886453</v>
+        <v>0.9000958750780547</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5159169161091697</v>
+        <v>0.8910492508907584</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5923285070011669</v>
+        <v>0.8932079631454063</v>
       </c>
       <c r="F31" t="n">
-        <v>0.9474537346464793</v>
+        <v>0.9105998586609055</v>
       </c>
       <c r="G31" t="n">
-        <v>1.078547923018934</v>
+        <v>1.012270837460969</v>
       </c>
       <c r="H31" t="n">
-        <v>1.179579313023547</v>
+        <v>1.158510313205837</v>
       </c>
       <c r="I31" t="n">
-        <v>1.202759933557879</v>
+        <v>1.314509528543109</v>
       </c>
       <c r="J31" t="n">
-        <v>1.156801821462648</v>
+        <v>1.416284678445879</v>
       </c>
       <c r="K31" t="n">
-        <v>1.102388943043829</v>
+        <v>1.423587856052446</v>
       </c>
       <c r="L31" t="n">
-        <v>1.054786375758301</v>
+        <v>1.441968094920279</v>
       </c>
       <c r="M31" t="n">
-        <v>1.021022909530092</v>
+        <v>1.431148587513198</v>
       </c>
       <c r="N31" t="n">
-        <v>0.9927284408030668</v>
+        <v>1.414888479313277</v>
       </c>
       <c r="O31" t="n">
-        <v>0.9860155480149131</v>
+        <v>1.404486307984056</v>
       </c>
       <c r="P31" t="n">
-        <v>0.9797220579845014</v>
+        <v>1.393613891770967</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.9791020860059347</v>
+        <v>1.394133762634534</v>
       </c>
       <c r="R31" t="n">
-        <v>0.9808898691039977</v>
+        <v>1.396561647073197</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7.017038286703823</v>
+        <v>70.04248435644998</v>
       </c>
       <c r="B32" t="n">
-        <v>0.4331518099430794</v>
+        <v>0.9155717115349616</v>
       </c>
       <c r="C32" t="n">
-        <v>0.449673310494435</v>
+        <v>0.9244259290667014</v>
       </c>
       <c r="D32" t="n">
-        <v>0.523931693760932</v>
+        <v>0.9152292918507039</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5703529251628491</v>
+        <v>0.9163293225071032</v>
       </c>
       <c r="F32" t="n">
-        <v>0.7902003573183002</v>
+        <v>0.9328270855970803</v>
       </c>
       <c r="G32" t="n">
-        <v>0.9637065877460986</v>
+        <v>1.008859641537164</v>
       </c>
       <c r="H32" t="n">
-        <v>1.128422907237454</v>
+        <v>1.143449110797898</v>
       </c>
       <c r="I32" t="n">
-        <v>1.170511058005679</v>
+        <v>1.304589801794256</v>
       </c>
       <c r="J32" t="n">
-        <v>1.159007099165276</v>
+        <v>1.381876857243773</v>
       </c>
       <c r="K32" t="n">
-        <v>1.102435718622854</v>
+        <v>1.405545537585053</v>
       </c>
       <c r="L32" t="n">
-        <v>1.055598183664111</v>
+        <v>1.429554960965303</v>
       </c>
       <c r="M32" t="n">
-        <v>1.025062509597221</v>
+        <v>1.416374011415749</v>
       </c>
       <c r="N32" t="n">
-        <v>1.00857906577574</v>
+        <v>1.40968107369687</v>
       </c>
       <c r="O32" t="n">
-        <v>0.9965912434691342</v>
+        <v>1.430350154645427</v>
       </c>
       <c r="P32" t="n">
-        <v>0.9943820756227172</v>
+        <v>1.437030953938224</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.9921152611788562</v>
+        <v>1.439366416601693</v>
       </c>
       <c r="R32" t="n">
-        <v>0.9912761718480519</v>
+        <v>1.439643162009105</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>9.426684551178845</v>
+        <v>87.13786733102222</v>
       </c>
       <c r="B33" t="n">
-        <v>0.455488648571577</v>
+        <v>0.9467413809551265</v>
       </c>
       <c r="C33" t="n">
-        <v>0.4767424038584759</v>
+        <v>0.9508356316906728</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5294776127237882</v>
+        <v>0.9415358784134573</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5549306216680346</v>
+        <v>0.9420315506607251</v>
       </c>
       <c r="F33" t="n">
-        <v>0.65985476956614</v>
+        <v>0.9575262474624022</v>
       </c>
       <c r="G33" t="n">
-        <v>0.8880585864188587</v>
+        <v>1.00884028459347</v>
       </c>
       <c r="H33" t="n">
-        <v>1.097848180275194</v>
+        <v>1.139573855324869</v>
       </c>
       <c r="I33" t="n">
-        <v>1.145925753077794</v>
+        <v>1.280600037473257</v>
       </c>
       <c r="J33" t="n">
-        <v>1.131840099920369</v>
+        <v>1.36751661829737</v>
       </c>
       <c r="K33" t="n">
-        <v>1.109743828128901</v>
+        <v>1.38867698886967</v>
       </c>
       <c r="L33" t="n">
-        <v>1.07842684654281</v>
+        <v>1.405054648232258</v>
       </c>
       <c r="M33" t="n">
-        <v>1.053217520868412</v>
+        <v>1.428455354673652</v>
       </c>
       <c r="N33" t="n">
-        <v>1.041893749611056</v>
+        <v>1.459067297911717</v>
       </c>
       <c r="O33" t="n">
-        <v>1.03072031473497</v>
+        <v>1.477437722196451</v>
       </c>
       <c r="P33" t="n">
-        <v>1.019645690538333</v>
+        <v>1.484526584842182</v>
       </c>
       <c r="Q33" t="n">
-        <v>1.011853042629318</v>
+        <v>1.486462220641694</v>
       </c>
       <c r="R33" t="n">
-        <v>1.006798646484459</v>
+        <v>1.484872416966359</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>12.66380173467402</v>
+        <v>108.4057482078677</v>
       </c>
       <c r="B34" t="n">
-        <v>0.481605676616977</v>
+        <v>0.9786654666958302</v>
       </c>
       <c r="C34" t="n">
-        <v>0.5056842095167617</v>
+        <v>0.9795261248476911</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5408707628659023</v>
+        <v>0.970463617488499</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5580073535404598</v>
+        <v>0.9703633736813162</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6155986906789388</v>
+        <v>0.9852940449798059</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8326056976244481</v>
+        <v>1.013894868434993</v>
       </c>
       <c r="H34" t="n">
-        <v>1.041821692752885</v>
+        <v>1.137046175239525</v>
       </c>
       <c r="I34" t="n">
-        <v>1.113558488036258</v>
+        <v>1.272467974118136</v>
       </c>
       <c r="J34" t="n">
-        <v>1.122584427027041</v>
+        <v>1.350043932805936</v>
       </c>
       <c r="K34" t="n">
-        <v>1.107252652977241</v>
+        <v>1.366621927443957</v>
       </c>
       <c r="L34" t="n">
-        <v>1.099131031038023</v>
+        <v>1.43334345792345</v>
       </c>
       <c r="M34" t="n">
-        <v>1.076108400560317</v>
+        <v>1.482727913150611</v>
       </c>
       <c r="N34" t="n">
-        <v>1.060307176359916</v>
+        <v>1.516011740013194</v>
       </c>
       <c r="O34" t="n">
-        <v>1.04521414271527</v>
+        <v>1.534186795690673</v>
       </c>
       <c r="P34" t="n">
-        <v>1.034692640515163</v>
+        <v>1.538776187471329</v>
       </c>
       <c r="Q34" t="n">
-        <v>1.028377821777827</v>
+        <v>1.537958862016337</v>
       </c>
       <c r="R34" t="n">
-        <v>1.021985895110555</v>
+        <v>1.533571015927145</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>17.01254279852586</v>
+        <v>134.8645153302234</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5109228419193235</v>
+        <v>1.011654307799899</v>
       </c>
       <c r="C35" t="n">
-        <v>0.5358141724975565</v>
+        <v>1.010847377996872</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5567638995302002</v>
+        <v>1.002259726682035</v>
       </c>
       <c r="E35" t="n">
-        <v>0.5702715021243413</v>
+        <v>1.001865297460894</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6181604880243261</v>
+        <v>1.016984403517928</v>
       </c>
       <c r="G35" t="n">
-        <v>0.8134261180388076</v>
+        <v>1.035224671387143</v>
       </c>
       <c r="H35" t="n">
-        <v>1.006248225599556</v>
+        <v>1.140136668696511</v>
       </c>
       <c r="I35" t="n">
-        <v>1.064223394857427</v>
+        <v>1.266407563763838</v>
       </c>
       <c r="J35" t="n">
-        <v>1.099678671534276</v>
+        <v>1.33393654417835</v>
       </c>
       <c r="K35" t="n">
-        <v>1.122300973779885</v>
+        <v>1.413481647780278</v>
       </c>
       <c r="L35" t="n">
-        <v>1.113637372516512</v>
+        <v>1.485779774532026</v>
       </c>
       <c r="M35" t="n">
-        <v>1.082521163980464</v>
+        <v>1.531228568995361</v>
       </c>
       <c r="N35" t="n">
-        <v>1.072535063555073</v>
+        <v>1.560199648636978</v>
       </c>
       <c r="O35" t="n">
-        <v>1.058572074849938</v>
+        <v>1.574716234307048</v>
       </c>
       <c r="P35" t="n">
-        <v>1.044733971797966</v>
+        <v>1.576680846561517</v>
       </c>
       <c r="Q35" t="n">
-        <v>1.036406362601291</v>
+        <v>1.573029296926287</v>
       </c>
       <c r="R35" t="n">
-        <v>1.030764740115881</v>
+        <v>1.566369208302691</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>22.85463864134988</v>
+        <v>167.7811167391214</v>
       </c>
       <c r="B36" t="n">
-        <v>0.5424405076432331</v>
+        <v>1.046105282447993</v>
       </c>
       <c r="C36" t="n">
-        <v>0.5666303671019479</v>
+        <v>1.045209940876572</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5747584384181843</v>
+        <v>1.037319064667173</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5856613083945894</v>
+        <v>1.037365383597937</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6153288766169971</v>
+        <v>1.048899516679695</v>
       </c>
       <c r="G36" t="n">
-        <v>0.7788153673517195</v>
+        <v>1.064581351724128</v>
       </c>
       <c r="H36" t="n">
-        <v>0.9566185279515058</v>
+        <v>1.148360471167159</v>
       </c>
       <c r="I36" t="n">
-        <v>1.039149886201996</v>
+        <v>1.267126084474045</v>
       </c>
       <c r="J36" t="n">
-        <v>1.09256405103493</v>
+        <v>1.377761101913775</v>
       </c>
       <c r="K36" t="n">
-        <v>1.115224734139147</v>
+        <v>1.462112201528674</v>
       </c>
       <c r="L36" t="n">
-        <v>1.113778838110334</v>
+        <v>1.528127498468045</v>
       </c>
       <c r="M36" t="n">
-        <v>1.097348352279845</v>
+        <v>1.572831173346346</v>
       </c>
       <c r="N36" t="n">
-        <v>1.079058789150732</v>
+        <v>1.601284023668563</v>
       </c>
       <c r="O36" t="n">
-        <v>1.067853049361587</v>
+        <v>1.614443380527331</v>
       </c>
       <c r="P36" t="n">
-        <v>1.058028585809209</v>
+        <v>1.615991315889384</v>
       </c>
       <c r="Q36" t="n">
-        <v>1.049795504608901</v>
+        <v>1.611423428295099</v>
       </c>
       <c r="R36" t="n">
-        <v>1.041379950279421</v>
+        <v>1.602491760731032</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>30.7029062975785</v>
+        <v>208.7317265427349</v>
       </c>
       <c r="B37" t="n">
-        <v>0.5756570401305598</v>
+        <v>1.082505388791398</v>
       </c>
       <c r="C37" t="n">
-        <v>0.5959073658191306</v>
+        <v>1.083202258460945</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5953727899693897</v>
+        <v>1.076131725779887</v>
       </c>
       <c r="E37" t="n">
-        <v>0.603394562553756</v>
+        <v>1.076935451565368</v>
       </c>
       <c r="F37" t="n">
-        <v>0.6185499535649569</v>
+        <v>1.082416570273528</v>
       </c>
       <c r="G37" t="n">
-        <v>0.7528003505887393</v>
+        <v>1.096034152235762</v>
       </c>
       <c r="H37" t="n">
-        <v>0.9178329006702124</v>
+        <v>1.171719224342616</v>
       </c>
       <c r="I37" t="n">
-        <v>1.004060846917367</v>
+        <v>1.309553509076854</v>
       </c>
       <c r="J37" t="n">
-        <v>1.073807979120849</v>
+        <v>1.422131191699312</v>
       </c>
       <c r="K37" t="n">
-        <v>1.113314661227202</v>
+        <v>1.500973961912587</v>
       </c>
       <c r="L37" t="n">
-        <v>1.119433301951641</v>
+        <v>1.571350895311687</v>
       </c>
       <c r="M37" t="n">
-        <v>1.096389097209391</v>
+        <v>1.610319803685487</v>
       </c>
       <c r="N37" t="n">
-        <v>1.069532759026314</v>
+        <v>1.632900123437406</v>
       </c>
       <c r="O37" t="n">
-        <v>1.056484545296774</v>
+        <v>1.641844559053833</v>
       </c>
       <c r="P37" t="n">
-        <v>1.045273518914932</v>
+        <v>1.640691644307231</v>
       </c>
       <c r="Q37" t="n">
-        <v>1.03535528010315</v>
+        <v>1.633416625491047</v>
       </c>
       <c r="R37" t="n">
-        <v>1.025716036902407</v>
+        <v>1.622221814251682</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>41.24626382901348</v>
+        <v>259.6772182250719</v>
       </c>
       <c r="B38" t="n">
-        <v>0.6101488984025074</v>
+        <v>1.12142878959603</v>
       </c>
       <c r="C38" t="n">
-        <v>0.6208911362779069</v>
+        <v>1.122081492825896</v>
       </c>
       <c r="D38" t="n">
-        <v>0.6185840843152635</v>
+        <v>1.119704274353285</v>
       </c>
       <c r="E38" t="n">
-        <v>0.6242659053110101</v>
+        <v>1.118990647565438</v>
       </c>
       <c r="F38" t="n">
-        <v>0.6368391352688864</v>
+        <v>1.121089656654838</v>
       </c>
       <c r="G38" t="n">
-        <v>0.7352031615986711</v>
+        <v>1.132602946169403</v>
       </c>
       <c r="H38" t="n">
-        <v>0.8860844829397502</v>
+        <v>1.21099454017414</v>
       </c>
       <c r="I38" t="n">
-        <v>0.9858477551013859</v>
+        <v>1.351189672301921</v>
       </c>
       <c r="J38" t="n">
-        <v>1.065125828741418</v>
+        <v>1.459751530096444</v>
       </c>
       <c r="K38" t="n">
-        <v>1.1022579731898</v>
+        <v>1.538837279026541</v>
       </c>
       <c r="L38" t="n">
-        <v>1.097776206692222</v>
+        <v>1.597997941771963</v>
       </c>
       <c r="M38" t="n">
-        <v>1.084670516305976</v>
+        <v>1.629502387955139</v>
       </c>
       <c r="N38" t="n">
-        <v>1.066910003646891</v>
+        <v>1.645987990430551</v>
       </c>
       <c r="O38" t="n">
-        <v>1.05196854755695</v>
+        <v>1.651765075278254</v>
       </c>
       <c r="P38" t="n">
-        <v>1.038560418623065</v>
+        <v>1.652123070528473</v>
       </c>
       <c r="Q38" t="n">
-        <v>1.028387764450846</v>
+        <v>1.645905435934273</v>
       </c>
       <c r="R38" t="n">
-        <v>1.020679968809754</v>
+        <v>1.635078701356749</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>55.41020330009481</v>
+        <v>323.0570588477636</v>
       </c>
       <c r="B39" t="n">
-        <v>0.6454818575089594</v>
+        <v>1.164424808183788</v>
       </c>
       <c r="C39" t="n">
-        <v>0.6480747585913258</v>
+        <v>1.165805936106489</v>
       </c>
       <c r="D39" t="n">
-        <v>0.6444058466251482</v>
+        <v>1.163364883782704</v>
       </c>
       <c r="E39" t="n">
-        <v>0.6480200336642261</v>
+        <v>1.163551661921615</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6582423337076756</v>
+        <v>1.167492890606939</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7227719098708513</v>
+        <v>1.176230408428658</v>
       </c>
       <c r="H39" t="n">
-        <v>0.8705278475938515</v>
+        <v>1.253327739666791</v>
       </c>
       <c r="I39" t="n">
-        <v>0.9721899860785397</v>
+        <v>1.389966672222414</v>
       </c>
       <c r="J39" t="n">
-        <v>1.048261243472579</v>
+        <v>1.493624221026003</v>
       </c>
       <c r="K39" t="n">
-        <v>1.082514825170847</v>
+        <v>1.560544018368817</v>
       </c>
       <c r="L39" t="n">
-        <v>1.094740044712552</v>
+        <v>1.613169256947059</v>
       </c>
       <c r="M39" t="n">
-        <v>1.080524549076629</v>
+        <v>1.641699887315835</v>
       </c>
       <c r="N39" t="n">
-        <v>1.058938801135282</v>
+        <v>1.656604231247536</v>
       </c>
       <c r="O39" t="n">
-        <v>1.049737710953587</v>
+        <v>1.662130824128161</v>
       </c>
       <c r="P39" t="n">
-        <v>1.05581328841047</v>
+        <v>1.660256442005224</v>
       </c>
       <c r="Q39" t="n">
-        <v>1.058549996632962</v>
+        <v>1.652077108960948</v>
       </c>
       <c r="R39" t="n">
-        <v>1.059138923004874</v>
+        <v>1.639868674059866</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>74.43803013251681</v>
+        <v>401.9061201622611</v>
       </c>
       <c r="B40" t="n">
-        <v>0.6809810012015657</v>
+        <v>1.212688439250157</v>
       </c>
       <c r="C40" t="n">
-        <v>0.6780130279251199</v>
+        <v>1.214051732446067</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6732460169422841</v>
+        <v>1.212088275329517</v>
       </c>
       <c r="E40" t="n">
-        <v>0.6753336497721345</v>
+        <v>1.21377840308928</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6840641020124496</v>
+        <v>1.2199568332378</v>
       </c>
       <c r="G40" t="n">
-        <v>0.7235191863767177</v>
+        <v>1.230927104071659</v>
       </c>
       <c r="H40" t="n">
-        <v>0.8625194148816397</v>
+        <v>1.294631883976065</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9597192217230051</v>
+        <v>1.424345250584319</v>
       </c>
       <c r="J40" t="n">
-        <v>1.034722712996596</v>
+        <v>1.516558948121224</v>
       </c>
       <c r="K40" t="n">
-        <v>1.071751584105683</v>
+        <v>1.582160998247127</v>
       </c>
       <c r="L40" t="n">
-        <v>1.072588145060508</v>
+        <v>1.627613980278141</v>
       </c>
       <c r="M40" t="n">
-        <v>1.078310922923118</v>
+        <v>1.648585239073881</v>
       </c>
       <c r="N40" t="n">
-        <v>1.102546271193743</v>
+        <v>1.655221922208677</v>
       </c>
       <c r="O40" t="n">
-        <v>1.110821769520903</v>
+        <v>1.6543582503956</v>
       </c>
       <c r="P40" t="n">
-        <v>1.114131905182496</v>
+        <v>1.651163164872976</v>
       </c>
       <c r="Q40" t="n">
-        <v>1.114093121457188</v>
+        <v>1.643856857531413</v>
       </c>
       <c r="R40" t="n">
-        <v>1.112865003653425</v>
+        <v>1.63206882777374</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="B41" t="n">
-        <v>0.7150718142464789</v>
+        <v>1.26607975253477</v>
       </c>
       <c r="C41" t="n">
-        <v>0.7111457707346283</v>
+        <v>1.267633628863605</v>
       </c>
       <c r="D41" t="n">
-        <v>0.7056680453256241</v>
+        <v>1.266704959308755</v>
       </c>
       <c r="E41" t="n">
-        <v>0.706946428226514</v>
+        <v>1.270473617481034</v>
       </c>
       <c r="F41" t="n">
-        <v>0.7144167252700651</v>
+        <v>1.279249159190819</v>
       </c>
       <c r="G41" t="n">
-        <v>0.7386929050745622</v>
+        <v>1.292823555573148</v>
       </c>
       <c r="H41" t="n">
-        <v>0.8646441774386795</v>
+        <v>1.336486498221441</v>
       </c>
       <c r="I41" t="n">
-        <v>0.9573089869699658</v>
+        <v>1.4574194425836</v>
       </c>
       <c r="J41" t="n">
-        <v>1.020625685367302</v>
+        <v>1.542030613773756</v>
       </c>
       <c r="K41" t="n">
-        <v>1.047137847459548</v>
+        <v>1.593237095320488</v>
       </c>
       <c r="L41" t="n">
-        <v>1.088714333780024</v>
+        <v>1.622483940791839</v>
       </c>
       <c r="M41" t="n">
-        <v>1.13814951061262</v>
+        <v>1.63897419052592</v>
       </c>
       <c r="N41" t="n">
-        <v>1.164756278268978</v>
+        <v>1.647506398184633</v>
       </c>
       <c r="O41" t="n">
-        <v>1.172608459179933</v>
+        <v>1.650511012654125</v>
       </c>
       <c r="P41" t="n">
-        <v>1.175299287675534</v>
+        <v>1.647736499932162</v>
       </c>
       <c r="Q41" t="n">
-        <v>1.173992029244687</v>
+        <v>1.639612816836155</v>
       </c>
       <c r="R41" t="n">
-        <v>1.171640020163526</v>
+        <v>1.62767486244848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added makefile for easibility
</commit_message>
<xml_diff>
--- a/beta_bruteforce.xlsx
+++ b/beta_bruteforce.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,117 +441,137 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>3x3</t>
+          <t>47x47</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>5x5</t>
+          <t>49x49</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>7x7</t>
+          <t>51x51</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>9x9</t>
+          <t>53x53</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>11x11</t>
+          <t>55x55</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>13x13</t>
+          <t>57x57</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15x15</t>
+          <t>59x59</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>17x17</t>
+          <t>61x61</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>19x19</t>
+          <t>63x63</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>21x21</t>
+          <t>65x65</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>23x23</t>
+          <t>67x67</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>25x25</t>
+          <t>69x69</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>27x27</t>
+          <t>71x71</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>29x29</t>
+          <t>73x73</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>31x31</t>
+          <t>75x75</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>33x33</t>
+          <t>77x77</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>35x35</t>
+          <t>79x79</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>37x37</t>
+          <t>81x81</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>39x39</t>
+          <t>83x83</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>41x41</t>
+          <t>85x85</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>43x43</t>
+          <t>87x87</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>45x45</t>
+          <t>89x89</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>47x47</t>
+          <t>91x91</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>93x93</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>95x95</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>97x97</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>99x99</t>
         </is>
       </c>
     </row>
@@ -560,2959 +580,3439 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7831001125092271</v>
+        <v>1.391666725565063</v>
       </c>
       <c r="C2" t="n">
-        <v>1.148846839329306</v>
+        <v>1.380251019660726</v>
       </c>
       <c r="D2" t="n">
-        <v>1.503823738530419</v>
+        <v>1.361527387510303</v>
       </c>
       <c r="E2" t="n">
-        <v>2.50494662615715</v>
+        <v>1.343060922448986</v>
       </c>
       <c r="F2" t="n">
-        <v>2.78355286812213</v>
+        <v>1.324205161181494</v>
       </c>
       <c r="G2" t="n">
-        <v>2.238695968823255</v>
+        <v>1.309083380003792</v>
       </c>
       <c r="H2" t="n">
-        <v>1.834536455505766</v>
+        <v>1.298126659422457</v>
       </c>
       <c r="I2" t="n">
-        <v>1.793514534280072</v>
+        <v>1.285118907424726</v>
       </c>
       <c r="J2" t="n">
-        <v>1.815387995360042</v>
+        <v>1.275676254861748</v>
       </c>
       <c r="K2" t="n">
-        <v>1.645065528638155</v>
+        <v>1.273820909882964</v>
       </c>
       <c r="L2" t="n">
-        <v>1.545665899011534</v>
+        <v>1.27093237222527</v>
       </c>
       <c r="M2" t="n">
-        <v>1.489035108090599</v>
+        <v>1.263657272299489</v>
       </c>
       <c r="N2" t="n">
-        <v>1.467090617552357</v>
+        <v>1.253677939860731</v>
       </c>
       <c r="O2" t="n">
-        <v>1.460552857654857</v>
+        <v>1.243972341221691</v>
       </c>
       <c r="P2" t="n">
-        <v>1.454505225996604</v>
+        <v>1.237092134936947</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.451493800321665</v>
+        <v>1.231822984316377</v>
       </c>
       <c r="R2" t="n">
-        <v>1.434540879229746</v>
+        <v>1.226540676578448</v>
       </c>
       <c r="S2" t="n">
-        <v>1.423877874638122</v>
+        <v>1.221509561249236</v>
       </c>
       <c r="T2" t="n">
-        <v>1.408503789469754</v>
+        <v>1.214188112228254</v>
       </c>
       <c r="U2" t="n">
-        <v>1.398632990770455</v>
+        <v>1.206497744387678</v>
       </c>
       <c r="V2" t="n">
-        <v>1.395465918267234</v>
+        <v>1.206633547738782</v>
       </c>
       <c r="W2" t="n">
-        <v>1.396731450037917</v>
+        <v>1.203073142168966</v>
       </c>
       <c r="X2" t="n">
-        <v>1.391666725565063</v>
+        <v>1.202174158913606</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>1.201464837488996</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1.196723348366251</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1.195156772022091</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1.193627443272793</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1215183306378339</v>
+        <v>0.1125335582600765</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7666317684188827</v>
+        <v>1.362273414219913</v>
       </c>
       <c r="C3" t="n">
-        <v>1.071599684506793</v>
+        <v>1.350026305695135</v>
       </c>
       <c r="D3" t="n">
-        <v>1.472482816300622</v>
+        <v>1.330322279856254</v>
       </c>
       <c r="E3" t="n">
-        <v>2.385485326359708</v>
+        <v>1.311271094121367</v>
       </c>
       <c r="F3" t="n">
-        <v>2.62736061302224</v>
+        <v>1.291617956335165</v>
       </c>
       <c r="G3" t="n">
-        <v>2.143334557380776</v>
+        <v>1.275024957939176</v>
       </c>
       <c r="H3" t="n">
-        <v>1.840154144706678</v>
+        <v>1.263368793207016</v>
       </c>
       <c r="I3" t="n">
-        <v>1.686419702139848</v>
+        <v>1.250058760491378</v>
       </c>
       <c r="J3" t="n">
-        <v>1.732612770393904</v>
+        <v>1.240524377830418</v>
       </c>
       <c r="K3" t="n">
-        <v>1.572563716013656</v>
+        <v>1.237909779506308</v>
       </c>
       <c r="L3" t="n">
-        <v>1.490760674043389</v>
+        <v>1.234449591755939</v>
       </c>
       <c r="M3" t="n">
-        <v>1.412375315460146</v>
+        <v>1.226529013167529</v>
       </c>
       <c r="N3" t="n">
-        <v>1.387222493044151</v>
+        <v>1.216456742036969</v>
       </c>
       <c r="O3" t="n">
-        <v>1.37644982041391</v>
+        <v>1.206466012077908</v>
       </c>
       <c r="P3" t="n">
-        <v>1.379194096404084</v>
+        <v>1.199593069714065</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.381956123877986</v>
+        <v>1.193613175375261</v>
       </c>
       <c r="R3" t="n">
-        <v>1.372030045395356</v>
+        <v>1.187881032287357</v>
       </c>
       <c r="S3" t="n">
-        <v>1.36954786306636</v>
+        <v>1.182760347869939</v>
       </c>
       <c r="T3" t="n">
-        <v>1.360487697300128</v>
+        <v>1.175642729582819</v>
       </c>
       <c r="U3" t="n">
-        <v>1.351291307479445</v>
+        <v>1.168395936377129</v>
       </c>
       <c r="V3" t="n">
-        <v>1.347434971279346</v>
+        <v>1.167973741291894</v>
       </c>
       <c r="W3" t="n">
-        <v>1.347111100109402</v>
+        <v>1.163612392511821</v>
       </c>
       <c r="X3" t="n">
-        <v>1.341736307796814</v>
+        <v>1.1621386247184</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1.160977024377647</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1.156158700513508</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1.154607059951354</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1.152985309180884</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1476670468100591</v>
+        <v>0.1266380173467403</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7489064305216915</v>
+        <v>1.330219042544425</v>
       </c>
       <c r="C4" t="n">
-        <v>1.018592938547337</v>
+        <v>1.317214944667543</v>
       </c>
       <c r="D4" t="n">
-        <v>1.42717582242552</v>
+        <v>1.296561621154446</v>
       </c>
       <c r="E4" t="n">
-        <v>2.292335311355665</v>
+        <v>1.276973299954472</v>
       </c>
       <c r="F4" t="n">
-        <v>2.462930409198777</v>
+        <v>1.256540290638099</v>
       </c>
       <c r="G4" t="n">
-        <v>2.117849028723439</v>
+        <v>1.238578099947799</v>
       </c>
       <c r="H4" t="n">
-        <v>1.874186154537032</v>
+        <v>1.226306868813146</v>
       </c>
       <c r="I4" t="n">
-        <v>1.631667021285835</v>
+        <v>1.212793705141704</v>
       </c>
       <c r="J4" t="n">
-        <v>1.63919806495932</v>
+        <v>1.203120817929258</v>
       </c>
       <c r="K4" t="n">
-        <v>1.537820364306332</v>
+        <v>1.19965496641733</v>
       </c>
       <c r="L4" t="n">
-        <v>1.456693149715377</v>
+        <v>1.195565493370996</v>
       </c>
       <c r="M4" t="n">
-        <v>1.37203037639783</v>
+        <v>1.187219518650151</v>
       </c>
       <c r="N4" t="n">
-        <v>1.342481424815351</v>
+        <v>1.177155223450674</v>
       </c>
       <c r="O4" t="n">
-        <v>1.328040519240659</v>
+        <v>1.166964909077877</v>
       </c>
       <c r="P4" t="n">
-        <v>1.328524177007316</v>
+        <v>1.160105706763558</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.330277080379001</v>
+        <v>1.153378734711036</v>
       </c>
       <c r="R4" t="n">
-        <v>1.31907453131044</v>
+        <v>1.147299481026447</v>
       </c>
       <c r="S4" t="n">
-        <v>1.315733156155525</v>
+        <v>1.14210930187246</v>
       </c>
       <c r="T4" t="n">
-        <v>1.305468423028992</v>
+        <v>1.135288619706147</v>
       </c>
       <c r="U4" t="n">
-        <v>1.296732261001594</v>
+        <v>1.128411417699704</v>
       </c>
       <c r="V4" t="n">
-        <v>1.292366386854799</v>
+        <v>1.127301035624248</v>
       </c>
       <c r="W4" t="n">
-        <v>1.290553406058115</v>
+        <v>1.12214365836436</v>
       </c>
       <c r="X4" t="n">
-        <v>1.284663309741296</v>
+        <v>1.120089400791689</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1.118533158033963</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>1.113626745275653</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1.112021558981143</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>1.110414788449739</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1794425301857725</v>
+        <v>0.1425102670302998</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7300187067556217</v>
+        <v>1.29556984034276</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9632053949141165</v>
+        <v>1.281810543339283</v>
       </c>
       <c r="D5" t="n">
-        <v>1.366023235235854</v>
+        <v>1.260303741819814</v>
       </c>
       <c r="E5" t="n">
-        <v>2.199585293139992</v>
+        <v>1.240204006424952</v>
       </c>
       <c r="F5" t="n">
-        <v>2.2911884949176</v>
+        <v>1.219033978018311</v>
       </c>
       <c r="G5" t="n">
-        <v>2.177338859590326</v>
+        <v>1.199913989349086</v>
       </c>
       <c r="H5" t="n">
-        <v>1.92061476675646</v>
+        <v>1.187099819424</v>
       </c>
       <c r="I5" t="n">
-        <v>1.658809225986925</v>
+        <v>1.173435180582203</v>
       </c>
       <c r="J5" t="n">
-        <v>1.544432014787136</v>
+        <v>1.163623281530606</v>
       </c>
       <c r="K5" t="n">
-        <v>1.495193723982464</v>
+        <v>1.159323757981754</v>
       </c>
       <c r="L5" t="n">
-        <v>1.414955048191554</v>
+        <v>1.154691662842465</v>
       </c>
       <c r="M5" t="n">
-        <v>1.324684802529731</v>
+        <v>1.145940118135258</v>
       </c>
       <c r="N5" t="n">
-        <v>1.291085228109498</v>
+        <v>1.135988650056756</v>
       </c>
       <c r="O5" t="n">
-        <v>1.272972603785315</v>
+        <v>1.126437938534138</v>
       </c>
       <c r="P5" t="n">
-        <v>1.27078428502552</v>
+        <v>1.129793921336886</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.271295798844304</v>
+        <v>1.124901056290381</v>
       </c>
       <c r="R5" t="n">
-        <v>1.258935846815606</v>
+        <v>1.124344551687333</v>
       </c>
       <c r="S5" t="n">
-        <v>1.254756692274444</v>
+        <v>1.120776840830256</v>
       </c>
       <c r="T5" t="n">
-        <v>1.243635475790252</v>
+        <v>1.117610099635326</v>
       </c>
       <c r="U5" t="n">
-        <v>1.235486320431945</v>
+        <v>1.115489031774109</v>
       </c>
       <c r="V5" t="n">
-        <v>1.230719554557529</v>
+        <v>1.110334583170521</v>
       </c>
       <c r="W5" t="n">
-        <v>1.227660735928597</v>
+        <v>1.110690943141549</v>
       </c>
       <c r="X5" t="n">
-        <v>1.221078877809801</v>
+        <v>1.114536518546045</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>1.117329192411341</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1.115089772570449</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1.107506639726713</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>1.100359917399989</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.2180555671360418</v>
+        <v>0.160371874375133</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7101240329677433</v>
+        <v>1.2584735850388</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9065089459737148</v>
+        <v>1.244015784597722</v>
       </c>
       <c r="D6" t="n">
-        <v>1.353774691864825</v>
+        <v>1.221736852685866</v>
       </c>
       <c r="E6" t="n">
-        <v>2.091843519434213</v>
+        <v>1.201208001539053</v>
       </c>
       <c r="F6" t="n">
-        <v>2.113241510484543</v>
+        <v>1.179483610060998</v>
       </c>
       <c r="G6" t="n">
-        <v>2.22186881551599</v>
+        <v>1.159317255195429</v>
       </c>
       <c r="H6" t="n">
-        <v>1.962885196053409</v>
+        <v>1.146051911207776</v>
       </c>
       <c r="I6" t="n">
-        <v>1.699729358559584</v>
+        <v>1.132212650113589</v>
       </c>
       <c r="J6" t="n">
-        <v>1.466898928506852</v>
+        <v>1.122303629752501</v>
       </c>
       <c r="K6" t="n">
-        <v>1.44447133581197</v>
+        <v>1.117204850536681</v>
       </c>
       <c r="L6" t="n">
-        <v>1.365534434478543</v>
+        <v>1.114117555845527</v>
       </c>
       <c r="M6" t="n">
-        <v>1.270774278511244</v>
+        <v>1.123204151138965</v>
       </c>
       <c r="N6" t="n">
-        <v>1.23348982722632</v>
+        <v>1.124370119540642</v>
       </c>
       <c r="O6" t="n">
-        <v>1.211863671249068</v>
+        <v>1.133014712675626</v>
       </c>
       <c r="P6" t="n">
-        <v>1.206680518289309</v>
+        <v>1.13564066833899</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.205703432771247</v>
+        <v>1.129634447834513</v>
       </c>
       <c r="R6" t="n">
-        <v>1.192231272740295</v>
+        <v>1.12846075875309</v>
       </c>
       <c r="S6" t="n">
-        <v>1.187375618300404</v>
+        <v>1.124339179536814</v>
       </c>
       <c r="T6" t="n">
-        <v>1.17587880963569</v>
+        <v>1.121052184940835</v>
       </c>
       <c r="U6" t="n">
-        <v>1.168165458543733</v>
+        <v>1.118859792998674</v>
       </c>
       <c r="V6" t="n">
-        <v>1.163243744959495</v>
+        <v>1.113453943810245</v>
       </c>
       <c r="W6" t="n">
-        <v>1.15918284305138</v>
+        <v>1.113575401121585</v>
       </c>
       <c r="X6" t="n">
-        <v>1.151915568527159</v>
+        <v>1.116912944359263</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1.119071571670884</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1.116297129887897</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1.108339611647978</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1.100828672480458</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.264977485046579</v>
+        <v>0.180472176682717</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6893980666074371</v>
+        <v>1.219118431115152</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8496716949998895</v>
+        <v>1.204044893960895</v>
       </c>
       <c r="D7" t="n">
-        <v>1.343411530007145</v>
+        <v>1.181114002523172</v>
       </c>
       <c r="E7" t="n">
-        <v>1.971296955323899</v>
+        <v>1.160222945798015</v>
       </c>
       <c r="F7" t="n">
-        <v>1.930243522315791</v>
+        <v>1.137967635640107</v>
       </c>
       <c r="G7" t="n">
-        <v>2.250518763463447</v>
+        <v>1.116937015275211</v>
       </c>
       <c r="H7" t="n">
-        <v>1.998316773832691</v>
+        <v>1.103369597555071</v>
       </c>
       <c r="I7" t="n">
-        <v>1.732079229920318</v>
+        <v>1.098792346608636</v>
       </c>
       <c r="J7" t="n">
-        <v>1.397441199346292</v>
+        <v>1.105993628936063</v>
       </c>
       <c r="K7" t="n">
-        <v>1.385502957487279</v>
+        <v>1.113263696598119</v>
       </c>
       <c r="L7" t="n">
-        <v>1.308611069180693</v>
+        <v>1.118186607978916</v>
       </c>
       <c r="M7" t="n">
-        <v>1.210779035350832</v>
+        <v>1.126658208799508</v>
       </c>
       <c r="N7" t="n">
-        <v>1.170414028119845</v>
+        <v>1.127271384679636</v>
       </c>
       <c r="O7" t="n">
-        <v>1.145541759217197</v>
+        <v>1.135190328970347</v>
       </c>
       <c r="P7" t="n">
-        <v>1.137227092692379</v>
+        <v>1.13704353914335</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.135521971112714</v>
+        <v>1.130237048637166</v>
       </c>
       <c r="R7" t="n">
-        <v>1.148328200128779</v>
+        <v>1.130742578679611</v>
       </c>
       <c r="S7" t="n">
-        <v>1.161652895705415</v>
+        <v>1.125658180781593</v>
       </c>
       <c r="T7" t="n">
-        <v>1.151928618205274</v>
+        <v>1.122692152372526</v>
       </c>
       <c r="U7" t="n">
-        <v>1.15192700178791</v>
+        <v>1.122892692812313</v>
       </c>
       <c r="V7" t="n">
-        <v>1.132378939418128</v>
+        <v>1.118196396019668</v>
       </c>
       <c r="W7" t="n">
-        <v>1.120920517634809</v>
+        <v>1.118210732704785</v>
       </c>
       <c r="X7" t="n">
-        <v>1.134462624778733</v>
+        <v>1.119715103662106</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1.119759555457934</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1.115928967583262</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>1.105407351602618</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>1.097877427557493</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.3219962163947186</v>
+        <v>0.2030917620904736</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6680567718424141</v>
+        <v>1.177707056838351</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7939565904732727</v>
+        <v>1.162103883485194</v>
       </c>
       <c r="D8" t="n">
-        <v>1.330289780085141</v>
+        <v>1.138648390125332</v>
       </c>
       <c r="E8" t="n">
-        <v>1.837356098204149</v>
+        <v>1.12727090123386</v>
       </c>
       <c r="F8" t="n">
-        <v>1.743446175401685</v>
+        <v>1.115962745268321</v>
       </c>
       <c r="G8" t="n">
-        <v>2.262681390913042</v>
+        <v>1.108419715449406</v>
       </c>
       <c r="H8" t="n">
-        <v>2.024182461708139</v>
+        <v>1.103276860490793</v>
       </c>
       <c r="I8" t="n">
-        <v>1.753713729365775</v>
+        <v>1.109317055990896</v>
       </c>
       <c r="J8" t="n">
-        <v>1.351441326390842</v>
+        <v>1.115304221645333</v>
       </c>
       <c r="K8" t="n">
-        <v>1.31856453785759</v>
+        <v>1.122192182325633</v>
       </c>
       <c r="L8" t="n">
-        <v>1.244620986530471</v>
+        <v>1.123839376471712</v>
       </c>
       <c r="M8" t="n">
-        <v>1.145478801869934</v>
+        <v>1.127304258506018</v>
       </c>
       <c r="N8" t="n">
-        <v>1.106533465211376</v>
+        <v>1.126354237441116</v>
       </c>
       <c r="O8" t="n">
-        <v>1.116253638699904</v>
+        <v>1.134566902729844</v>
       </c>
       <c r="P8" t="n">
-        <v>1.139285209046309</v>
+        <v>1.137835610785599</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.145690139327465</v>
+        <v>1.133826782219583</v>
       </c>
       <c r="R8" t="n">
-        <v>1.151474946705016</v>
+        <v>1.133801227343741</v>
       </c>
       <c r="S8" t="n">
-        <v>1.166986585533869</v>
+        <v>1.128257786590225</v>
       </c>
       <c r="T8" t="n">
-        <v>1.164717674071811</v>
+        <v>1.125310919216916</v>
       </c>
       <c r="U8" t="n">
-        <v>1.164051072981924</v>
+        <v>1.125286906351872</v>
       </c>
       <c r="V8" t="n">
-        <v>1.143484935105633</v>
+        <v>1.120279786089031</v>
       </c>
       <c r="W8" t="n">
-        <v>1.130117462378889</v>
+        <v>1.119689023913071</v>
       </c>
       <c r="X8" t="n">
-        <v>1.140838023503059</v>
+        <v>1.120539446069679</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>1.119903524982801</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1.115555513586811</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1.104964624086529</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>1.09737045578891</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.3912844268798491</v>
+        <v>0.2285463864134991</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6463796698320666</v>
+        <v>1.134506899045108</v>
       </c>
       <c r="C9" t="n">
-        <v>0.74069100670239</v>
+        <v>1.14380682692746</v>
       </c>
       <c r="D9" t="n">
-        <v>1.285595892488622</v>
+        <v>1.149648989781855</v>
       </c>
       <c r="E9" t="n">
-        <v>1.689411615125876</v>
+        <v>1.139247458813984</v>
       </c>
       <c r="F9" t="n">
-        <v>1.762732047827001</v>
+        <v>1.121315999685416</v>
       </c>
       <c r="G9" t="n">
-        <v>2.259895089094848</v>
+        <v>1.115075517942015</v>
       </c>
       <c r="H9" t="n">
-        <v>2.038032915863415</v>
+        <v>1.110711550778307</v>
       </c>
       <c r="I9" t="n">
-        <v>1.762546127000405</v>
+        <v>1.115591093774399</v>
       </c>
       <c r="J9" t="n">
-        <v>1.375228699954406</v>
+        <v>1.120331025668406</v>
       </c>
       <c r="K9" t="n">
-        <v>1.244186476819496</v>
+        <v>1.126758936651095</v>
       </c>
       <c r="L9" t="n">
-        <v>1.174260679355837</v>
+        <v>1.127414636645086</v>
       </c>
       <c r="M9" t="n">
-        <v>1.122185302492142</v>
+        <v>1.130009518485655</v>
       </c>
       <c r="N9" t="n">
-        <v>1.122710517186245</v>
+        <v>1.128208476913734</v>
       </c>
       <c r="O9" t="n">
-        <v>1.130201648244098</v>
+        <v>1.135548527095162</v>
       </c>
       <c r="P9" t="n">
-        <v>1.147637714817065</v>
+        <v>1.137946683504105</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.153580790632266</v>
+        <v>1.132729647162311</v>
       </c>
       <c r="R9" t="n">
-        <v>1.154766427601961</v>
+        <v>1.132108436118489</v>
       </c>
       <c r="S9" t="n">
-        <v>1.16819477128605</v>
+        <v>1.126137698529217</v>
       </c>
       <c r="T9" t="n">
-        <v>1.164988987009858</v>
+        <v>1.123195660172023</v>
       </c>
       <c r="U9" t="n">
-        <v>1.163286143030557</v>
+        <v>1.122864341043514</v>
       </c>
       <c r="V9" t="n">
-        <v>1.141650654310449</v>
+        <v>1.117496192789557</v>
       </c>
       <c r="W9" t="n">
-        <v>1.126320045609941</v>
+        <v>1.116383578340481</v>
       </c>
       <c r="X9" t="n">
-        <v>1.141220315789961</v>
+        <v>1.116461681303703</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>1.115192726304422</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1.110358714893937</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>1.099742060588741</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>1.092114778959936</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.4754823035902083</v>
+        <v>0.2571913809059345</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6247059965971362</v>
+        <v>1.132446154116701</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6912560556686719</v>
+        <v>1.153490239939049</v>
       </c>
       <c r="D10" t="n">
-        <v>1.227173888869291</v>
+        <v>1.158107454867705</v>
       </c>
       <c r="E10" t="n">
-        <v>1.527064255492173</v>
+        <v>1.14701974738586</v>
       </c>
       <c r="F10" t="n">
-        <v>1.80481870354551</v>
+        <v>1.128431057790189</v>
       </c>
       <c r="G10" t="n">
-        <v>2.241007883899707</v>
+        <v>1.118599783720547</v>
       </c>
       <c r="H10" t="n">
-        <v>2.037614120999093</v>
+        <v>1.113620261116743</v>
       </c>
       <c r="I10" t="n">
-        <v>1.75679815593645</v>
+        <v>1.117252897975104</v>
       </c>
       <c r="J10" t="n">
-        <v>1.385091068724583</v>
+        <v>1.120692311690939</v>
       </c>
       <c r="K10" t="n">
-        <v>1.222954450410763</v>
+        <v>1.126564204137375</v>
       </c>
       <c r="L10" t="n">
-        <v>1.172369185735014</v>
+        <v>1.126339883449717</v>
       </c>
       <c r="M10" t="n">
-        <v>1.13130970522985</v>
+        <v>1.127947361349477</v>
       </c>
       <c r="N10" t="n">
-        <v>1.126006464558013</v>
+        <v>1.125340581460431</v>
       </c>
       <c r="O10" t="n">
-        <v>1.130717516400041</v>
+        <v>1.131662911400843</v>
       </c>
       <c r="P10" t="n">
-        <v>1.142613871826815</v>
+        <v>1.133235067148201</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.14780295639251</v>
+        <v>1.126780378952794</v>
       </c>
       <c r="R10" t="n">
-        <v>1.145898386128511</v>
+        <v>1.125488194985518</v>
       </c>
       <c r="S10" t="n">
-        <v>1.155921303830935</v>
+        <v>1.119128710142323</v>
       </c>
       <c r="T10" t="n">
-        <v>1.151563920627497</v>
+        <v>1.116146551208895</v>
       </c>
       <c r="U10" t="n">
-        <v>1.148558744139846</v>
+        <v>1.115519769418182</v>
       </c>
       <c r="V10" t="n">
-        <v>1.125965849102066</v>
+        <v>1.109749780686093</v>
       </c>
       <c r="W10" t="n">
-        <v>1.125770414630622</v>
+        <v>1.108032623219682</v>
       </c>
       <c r="X10" t="n">
-        <v>1.162398740639201</v>
+        <v>1.10737451015771</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>1.105453036050235</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>1.100195434430493</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>1.089618047258782</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>1.086502565489902</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.5777981578011382</v>
+        <v>0.289426612471675</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6034726478095394</v>
+        <v>1.138822233840415</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6470309666956126</v>
+        <v>1.158841081598267</v>
       </c>
       <c r="D11" t="n">
-        <v>1.154285819297999</v>
+        <v>1.162128815993997</v>
       </c>
       <c r="E11" t="n">
-        <v>1.350386539292452</v>
+        <v>1.150344821379215</v>
       </c>
       <c r="F11" t="n">
-        <v>1.835609433435624</v>
+        <v>1.131095239229916</v>
       </c>
       <c r="G11" t="n">
-        <v>2.252645171681275</v>
+        <v>1.117299073599914</v>
       </c>
       <c r="H11" t="n">
-        <v>2.034625502684785</v>
+        <v>1.11166366462652</v>
       </c>
       <c r="I11" t="n">
-        <v>1.734992773438907</v>
+        <v>1.114052088882177</v>
       </c>
       <c r="J11" t="n">
-        <v>1.380851173366323</v>
+        <v>1.116196841294959</v>
       </c>
       <c r="K11" t="n">
-        <v>1.22931375360278</v>
+        <v>1.121484755099973</v>
       </c>
       <c r="L11" t="n">
-        <v>1.174803319016583</v>
+        <v>1.120261259809825</v>
       </c>
       <c r="M11" t="n">
-        <v>1.126944850409004</v>
+        <v>1.120983962950411</v>
       </c>
       <c r="N11" t="n">
-        <v>1.115584539614583</v>
+        <v>1.117529232253087</v>
       </c>
       <c r="O11" t="n">
-        <v>1.117076551311574</v>
+        <v>1.122815037190049</v>
       </c>
       <c r="P11" t="n">
-        <v>1.123537027324962</v>
+        <v>1.123491997379816</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.127653523999116</v>
+        <v>1.125365158155635</v>
       </c>
       <c r="R11" t="n">
-        <v>1.12289609012317</v>
+        <v>1.123643410475707</v>
       </c>
       <c r="S11" t="n">
-        <v>1.141337505214234</v>
+        <v>1.122581067161126</v>
       </c>
       <c r="T11" t="n">
-        <v>1.148409271480527</v>
+        <v>1.116592166148462</v>
       </c>
       <c r="U11" t="n">
-        <v>1.152622797798265</v>
+        <v>1.108081888071339</v>
       </c>
       <c r="V11" t="n">
-        <v>1.142684061429113</v>
+        <v>1.097557375350858</v>
       </c>
       <c r="W11" t="n">
-        <v>1.148737769383714</v>
+        <v>1.096674224093909</v>
       </c>
       <c r="X11" t="n">
-        <v>1.182811645251528</v>
+        <v>1.098802018095225</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>1.098800654172785</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>1.098647222756345</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1.099252557156784</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>1.101900529643243</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.7021306758161</v>
+        <v>0.3257020655659783</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5832118421954895</v>
+        <v>1.140816208481985</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6093134707822622</v>
+        <v>1.159670585689423</v>
       </c>
       <c r="D12" t="n">
-        <v>1.066664724247204</v>
+        <v>1.161554724618706</v>
       </c>
       <c r="E12" t="n">
-        <v>1.306242572732466</v>
+        <v>1.149035740264102</v>
       </c>
       <c r="F12" t="n">
-        <v>1.853374486987462</v>
+        <v>1.129182919641067</v>
       </c>
       <c r="G12" t="n">
-        <v>2.256275658998081</v>
+        <v>1.111039177198283</v>
       </c>
       <c r="H12" t="n">
-        <v>2.02075340190964</v>
+        <v>1.104712731839421</v>
       </c>
       <c r="I12" t="n">
-        <v>1.695936684335152</v>
+        <v>1.105793062931106</v>
       </c>
       <c r="J12" t="n">
-        <v>1.370862168680099</v>
+        <v>1.106626791180192</v>
       </c>
       <c r="K12" t="n">
-        <v>1.220272657932143</v>
+        <v>1.111265319607406</v>
       </c>
       <c r="L12" t="n">
-        <v>1.162497113914648</v>
+        <v>1.109175192633899</v>
       </c>
       <c r="M12" t="n">
-        <v>1.108570811107421</v>
+        <v>1.111067381095213</v>
       </c>
       <c r="N12" t="n">
-        <v>1.091188517619383</v>
+        <v>1.123069218036013</v>
       </c>
       <c r="O12" t="n">
-        <v>1.089159519939523</v>
+        <v>1.13265254568293</v>
       </c>
       <c r="P12" t="n">
-        <v>1.105294693574156</v>
+        <v>1.139099036850589</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.120044029503647</v>
+        <v>1.140928264787882</v>
       </c>
       <c r="R12" t="n">
-        <v>1.138501166536667</v>
+        <v>1.13835907034066</v>
       </c>
       <c r="S12" t="n">
-        <v>1.158742789867683</v>
+        <v>1.136541491048616</v>
       </c>
       <c r="T12" t="n">
-        <v>1.164488925202517</v>
+        <v>1.129776515820133</v>
       </c>
       <c r="U12" t="n">
-        <v>1.167159204482972</v>
+        <v>1.120265273187334</v>
       </c>
       <c r="V12" t="n">
-        <v>1.156335567261807</v>
+        <v>1.109623075149858</v>
       </c>
       <c r="W12" t="n">
-        <v>1.160455431580199</v>
+        <v>1.111084957074677</v>
       </c>
       <c r="X12" t="n">
-        <v>1.189876648901064</v>
+        <v>1.112593534136808</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>1.112093638576735</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>1.110746386628129</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>1.111150925829041</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>1.1133522977577</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.8532174761478657</v>
+        <v>0.3665241237079628</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5645696205140701</v>
+        <v>1.138282988528635</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5792163269019804</v>
+        <v>1.155736357555884</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9650418571672441</v>
+        <v>1.156191970653136</v>
       </c>
       <c r="E13" t="n">
-        <v>1.254346548345109</v>
+        <v>1.142933704340207</v>
       </c>
       <c r="F13" t="n">
-        <v>1.856434825288303</v>
+        <v>1.126193752632353</v>
       </c>
       <c r="G13" t="n">
-        <v>2.246996283215847</v>
+        <v>1.102144164227901</v>
       </c>
       <c r="H13" t="n">
-        <v>1.986718561741808</v>
+        <v>1.092668745730848</v>
       </c>
       <c r="I13" t="n">
-        <v>1.648729031188372</v>
+        <v>1.092400465499162</v>
       </c>
       <c r="J13" t="n">
-        <v>1.343772590573019</v>
+        <v>1.091913493680507</v>
       </c>
       <c r="K13" t="n">
-        <v>1.203389586295532</v>
+        <v>1.102701494216816</v>
       </c>
       <c r="L13" t="n">
-        <v>1.145212701460258</v>
+        <v>1.108398532551911</v>
       </c>
       <c r="M13" t="n">
-        <v>1.112750225808265</v>
+        <v>1.125044448602333</v>
       </c>
       <c r="N13" t="n">
-        <v>1.098074931319024</v>
+        <v>1.136350952755152</v>
       </c>
       <c r="O13" t="n">
-        <v>1.10633127298779</v>
+        <v>1.145501677830206</v>
       </c>
       <c r="P13" t="n">
-        <v>1.119474765717146</v>
+        <v>1.15131547845234</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.132867959597293</v>
+        <v>1.152291387389505</v>
       </c>
       <c r="R13" t="n">
-        <v>1.147844500459915</v>
+        <v>1.148878423798992</v>
       </c>
       <c r="S13" t="n">
-        <v>1.164964232665214</v>
+        <v>1.14629634378279</v>
       </c>
       <c r="T13" t="n">
-        <v>1.169060176558377</v>
+        <v>1.13879352094775</v>
       </c>
       <c r="U13" t="n">
-        <v>1.169988873734293</v>
+        <v>1.128358331400175</v>
       </c>
       <c r="V13" t="n">
-        <v>1.156759104808801</v>
+        <v>1.12057162577261</v>
       </c>
       <c r="W13" t="n">
-        <v>1.158509137181026</v>
+        <v>1.121692637228193</v>
       </c>
       <c r="X13" t="n">
-        <v>1.182677868074088</v>
+        <v>1.122577183429742</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>1.121592709607899</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>1.118587969217325</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>1.118767812236566</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>1.120506819608766</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.036815633725145</v>
+        <v>0.4124626382901352</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5482849315168011</v>
+        <v>1.146925194183593</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5658400034965227</v>
+        <v>1.156897959635849</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8523778638000696</v>
+        <v>1.165077552578012</v>
       </c>
       <c r="E14" t="n">
-        <v>1.18747027790348</v>
+        <v>1.157306732834796</v>
       </c>
       <c r="F14" t="n">
-        <v>1.843162220376479</v>
+        <v>1.145458780073998</v>
       </c>
       <c r="G14" t="n">
-        <v>2.211667524420066</v>
+        <v>1.120328958294039</v>
       </c>
       <c r="H14" t="n">
-        <v>1.931859775721297</v>
+        <v>1.102649476588793</v>
       </c>
       <c r="I14" t="n">
-        <v>1.608077748372142</v>
+        <v>1.090216939540422</v>
       </c>
       <c r="J14" t="n">
-        <v>1.356316814743787</v>
+        <v>1.100868276439414</v>
       </c>
       <c r="K14" t="n">
-        <v>1.224828337464586</v>
+        <v>1.11579575958896</v>
       </c>
       <c r="L14" t="n">
-        <v>1.165359108938548</v>
+        <v>1.119994642044707</v>
       </c>
       <c r="M14" t="n">
-        <v>1.116031681130157</v>
+        <v>1.134889483229402</v>
       </c>
       <c r="N14" t="n">
-        <v>1.109495945817936</v>
+        <v>1.145386262561055</v>
       </c>
       <c r="O14" t="n">
-        <v>1.114388799190964</v>
+        <v>1.153978893142427</v>
       </c>
       <c r="P14" t="n">
-        <v>1.122884361268365</v>
+        <v>1.159081210698546</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.13442527452864</v>
+        <v>1.15910632576735</v>
       </c>
       <c r="R14" t="n">
-        <v>1.145626952284495</v>
+        <v>1.154872804673575</v>
       </c>
       <c r="S14" t="n">
-        <v>1.15930201659543</v>
+        <v>1.151535288812203</v>
       </c>
       <c r="T14" t="n">
-        <v>1.161564577288703</v>
+        <v>1.143416502553139</v>
       </c>
       <c r="U14" t="n">
-        <v>1.160577370145293</v>
+        <v>1.13207068726628</v>
       </c>
       <c r="V14" t="n">
-        <v>1.157217023116551</v>
+        <v>1.127733464037022</v>
       </c>
       <c r="W14" t="n">
-        <v>1.161447395478106</v>
+        <v>1.128260563969116</v>
       </c>
       <c r="X14" t="n">
-        <v>1.185417819041752</v>
+        <v>1.128547925358143</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>1.127095477304266</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>1.122459613284243</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>1.121973625825281</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>1.123236577955401</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.259921049894873</v>
+        <v>0.4641588833612779</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5351376248329964</v>
+        <v>1.159003354445075</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5795189963496772</v>
+        <v>1.174535433133345</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7491710823339859</v>
+        <v>1.181018602737457</v>
       </c>
       <c r="E15" t="n">
-        <v>1.105859675904807</v>
+        <v>1.17262741957068</v>
       </c>
       <c r="F15" t="n">
-        <v>1.812035699602683</v>
+        <v>1.160394066120863</v>
       </c>
       <c r="G15" t="n">
-        <v>2.132396058971564</v>
+        <v>1.134225732101376</v>
       </c>
       <c r="H15" t="n">
-        <v>1.856016455556529</v>
+        <v>1.115001065092631</v>
       </c>
       <c r="I15" t="n">
-        <v>1.600355090941276</v>
+        <v>1.101271083273204</v>
       </c>
       <c r="J15" t="n">
-        <v>1.363091599626981</v>
+        <v>1.110319776667041</v>
       </c>
       <c r="K15" t="n">
-        <v>1.234091579928406</v>
+        <v>1.125080172727979</v>
       </c>
       <c r="L15" t="n">
-        <v>1.174008452549945</v>
+        <v>1.128644179086807</v>
       </c>
       <c r="M15" t="n">
-        <v>1.12165348512488</v>
+        <v>1.140357359441206</v>
       </c>
       <c r="N15" t="n">
-        <v>1.109904214189687</v>
+        <v>1.14996587836563</v>
       </c>
       <c r="O15" t="n">
-        <v>1.111070160570938</v>
+        <v>1.157897128708258</v>
       </c>
       <c r="P15" t="n">
-        <v>1.124175175220393</v>
+        <v>1.162199937139445</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.146721648696103</v>
+        <v>1.161185854023468</v>
       </c>
       <c r="R15" t="n">
-        <v>1.153533665788954</v>
+        <v>1.156176494461704</v>
       </c>
       <c r="S15" t="n">
-        <v>1.158427753364207</v>
+        <v>1.152133332929072</v>
       </c>
       <c r="T15" t="n">
-        <v>1.168472117398157</v>
+        <v>1.143453479676006</v>
       </c>
       <c r="U15" t="n">
-        <v>1.169690416608012</v>
+        <v>1.131316690147791</v>
       </c>
       <c r="V15" t="n">
-        <v>1.174393211123983</v>
+        <v>1.130639514532793</v>
       </c>
       <c r="W15" t="n">
-        <v>1.173833590941568</v>
+        <v>1.130644254243677</v>
       </c>
       <c r="X15" t="n">
-        <v>1.19567401394252</v>
+        <v>1.130295470924551</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>1.128413510512503</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>1.123556510099145</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>1.120524004347582</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>1.121337829569639</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.53103502718692</v>
+        <v>0.5223345074266842</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5258819184029228</v>
+        <v>1.173830070230189</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5829145766731306</v>
+        <v>1.187663398338032</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7386212899681994</v>
+        <v>1.192390067943055</v>
       </c>
       <c r="E16" t="n">
-        <v>1.01367025567389</v>
+        <v>1.183320159951989</v>
       </c>
       <c r="F16" t="n">
-        <v>1.758218235474021</v>
+        <v>1.170647709928577</v>
       </c>
       <c r="G16" t="n">
-        <v>2.041732098623904</v>
+        <v>1.143585451644015</v>
       </c>
       <c r="H16" t="n">
-        <v>1.759155816221109</v>
+        <v>1.122893906138799</v>
       </c>
       <c r="I16" t="n">
-        <v>1.580531372396599</v>
+        <v>1.108004506024713</v>
       </c>
       <c r="J16" t="n">
-        <v>1.355703254120926</v>
+        <v>1.115808051368373</v>
       </c>
       <c r="K16" t="n">
-        <v>1.239481164242721</v>
+        <v>1.130269595125799</v>
       </c>
       <c r="L16" t="n">
-        <v>1.171909708815533</v>
+        <v>1.133213306145241</v>
       </c>
       <c r="M16" t="n">
-        <v>1.129763129870796</v>
+        <v>1.141292222578002</v>
       </c>
       <c r="N16" t="n">
-        <v>1.110149487683132</v>
+        <v>1.149852530522601</v>
       </c>
       <c r="O16" t="n">
-        <v>1.100671604000164</v>
+        <v>1.157023334720226</v>
       </c>
       <c r="P16" t="n">
-        <v>1.135283819379471</v>
+        <v>1.160481573532553</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.156656670534349</v>
+        <v>1.1583547147531</v>
       </c>
       <c r="R16" t="n">
-        <v>1.164798111556121</v>
+        <v>1.152598802313859</v>
       </c>
       <c r="S16" t="n">
-        <v>1.172409820568126</v>
+        <v>1.147889841126019</v>
       </c>
       <c r="T16" t="n">
-        <v>1.182576142750507</v>
+        <v>1.138792404320633</v>
       </c>
       <c r="U16" t="n">
-        <v>1.181784275408349</v>
+        <v>1.13068956166362</v>
       </c>
       <c r="V16" t="n">
-        <v>1.184211558208037</v>
+        <v>1.129297537801069</v>
       </c>
       <c r="W16" t="n">
-        <v>1.180160696641648</v>
+        <v>1.128676530085501</v>
       </c>
       <c r="X16" t="n">
-        <v>1.195649363126711</v>
+        <v>1.127791532793404</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1.125471328154051</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>1.120427255696759</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1.114370541756645</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>1.114728992957815</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.860488206518051</v>
+        <v>0.5878016072274912</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5297924302467617</v>
+        <v>1.183990641474805</v>
       </c>
       <c r="C17" t="n">
-        <v>0.587151977945308</v>
+        <v>1.195961543935514</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7344452525395802</v>
+        <v>1.19885449216458</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9216897638437929</v>
+        <v>1.189100833705816</v>
       </c>
       <c r="F17" t="n">
-        <v>1.662710245736521</v>
+        <v>1.175994630666915</v>
       </c>
       <c r="G17" t="n">
-        <v>1.939347014339451</v>
+        <v>1.14814899235909</v>
       </c>
       <c r="H17" t="n">
-        <v>1.708048065131971</v>
+        <v>1.12620020472416</v>
       </c>
       <c r="I17" t="n">
-        <v>1.542461541353256</v>
+        <v>1.11021011241018</v>
       </c>
       <c r="J17" t="n">
-        <v>1.333796473628758</v>
+        <v>1.11717806176983</v>
       </c>
       <c r="K17" t="n">
-        <v>1.249276186957665</v>
+        <v>1.13122162733413</v>
       </c>
       <c r="L17" t="n">
-        <v>1.200790875795522</v>
+        <v>1.133541680541552</v>
       </c>
       <c r="M17" t="n">
-        <v>1.153925487524372</v>
+        <v>1.137540335318418</v>
       </c>
       <c r="N17" t="n">
-        <v>1.125571920132233</v>
+        <v>1.144931585325402</v>
       </c>
       <c r="O17" t="n">
-        <v>1.111698634047138</v>
+        <v>1.15124680129755</v>
       </c>
       <c r="P17" t="n">
-        <v>1.144657819439198</v>
+        <v>1.153771042041424</v>
       </c>
       <c r="Q17" t="n">
-        <v>1.165583556970342</v>
+        <v>1.150525423929976</v>
       </c>
       <c r="R17" t="n">
-        <v>1.169704626881268</v>
+        <v>1.144087028579412</v>
       </c>
       <c r="S17" t="n">
-        <v>1.174436212090579</v>
+        <v>1.138751646681527</v>
       </c>
       <c r="T17" t="n">
-        <v>1.182101808267464</v>
+        <v>1.129323636941893</v>
       </c>
       <c r="U17" t="n">
-        <v>1.179178428378609</v>
+        <v>1.125710143782116</v>
       </c>
       <c r="V17" t="n">
-        <v>1.178905450098675</v>
+        <v>1.123554812443462</v>
       </c>
       <c r="W17" t="n">
-        <v>1.171217731991528</v>
+        <v>1.122346886502039</v>
       </c>
       <c r="X17" t="n">
-        <v>1.182029233555352</v>
+        <v>1.120902366590155</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>1.118203300395219</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>1.113002094387238</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1.110801254964688</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>1.113782312989692</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2.26083421027451</v>
+        <v>0.6614740641230149</v>
       </c>
       <c r="B18" t="n">
-        <v>0.545498276182703</v>
+        <v>1.18918454836097</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5924915696936938</v>
+        <v>1.199158605046246</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7437274162040726</v>
+        <v>1.200220331117625</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8588814822456178</v>
+        <v>1.189770156992651</v>
       </c>
       <c r="F18" t="n">
-        <v>1.552572072647222</v>
+        <v>1.176235659409694</v>
       </c>
       <c r="G18" t="n">
-        <v>1.829922400516639</v>
+        <v>1.147784320422306</v>
       </c>
       <c r="H18" t="n">
-        <v>1.644728473675876</v>
+        <v>1.124666551095856</v>
       </c>
       <c r="I18" t="n">
-        <v>1.506285750699649</v>
+        <v>1.107784298300005</v>
       </c>
       <c r="J18" t="n">
-        <v>1.353418849848229</v>
+        <v>1.114308839195748</v>
       </c>
       <c r="K18" t="n">
-        <v>1.26466732867322</v>
+        <v>1.127777277633584</v>
       </c>
       <c r="L18" t="n">
-        <v>1.215644580159705</v>
+        <v>1.129520024690252</v>
       </c>
       <c r="M18" t="n">
-        <v>1.179562386098184</v>
+        <v>1.13229776312697</v>
       </c>
       <c r="N18" t="n">
-        <v>1.159336645926387</v>
+        <v>1.139915736024221</v>
       </c>
       <c r="O18" t="n">
-        <v>1.146319520369805</v>
+        <v>1.148538934199293</v>
       </c>
       <c r="P18" t="n">
-        <v>1.14599678879762</v>
+        <v>1.152102350136634</v>
       </c>
       <c r="Q18" t="n">
-        <v>1.171356733868333</v>
+        <v>1.149031708804522</v>
       </c>
       <c r="R18" t="n">
-        <v>1.175891593377261</v>
+        <v>1.144775053681289</v>
       </c>
       <c r="S18" t="n">
-        <v>1.182481936298605</v>
+        <v>1.138322207003838</v>
       </c>
       <c r="T18" t="n">
-        <v>1.18600222419068</v>
+        <v>1.130521497358448</v>
       </c>
       <c r="U18" t="n">
-        <v>1.183454823888993</v>
+        <v>1.118160208271699</v>
       </c>
       <c r="V18" t="n">
-        <v>1.186028262546382</v>
+        <v>1.113466914027369</v>
       </c>
       <c r="W18" t="n">
-        <v>1.180510212259532</v>
+        <v>1.111655534895677</v>
       </c>
       <c r="X18" t="n">
-        <v>1.190022210593722</v>
+        <v>1.112966431432481</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1.118709681041433</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>1.123000592855314</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>1.125507765035388</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>1.128010532220247</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2.747327990814638</v>
+        <v>0.7443803013251689</v>
       </c>
       <c r="B19" t="n">
-        <v>0.5630210185849838</v>
+        <v>1.189257832037528</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5988675870698489</v>
+        <v>1.197080395861509</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7382420726934542</v>
+        <v>1.196290157214871</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8604479440311671</v>
+        <v>1.185202031862162</v>
       </c>
       <c r="F19" t="n">
-        <v>1.441990456075882</v>
+        <v>1.171290433775514</v>
       </c>
       <c r="G19" t="n">
-        <v>1.711865320237357</v>
+        <v>1.142371871441016</v>
       </c>
       <c r="H19" t="n">
-        <v>1.579505475663572</v>
+        <v>1.118329724158713</v>
       </c>
       <c r="I19" t="n">
-        <v>1.52221140074249</v>
+        <v>1.106074682762701</v>
       </c>
       <c r="J19" t="n">
-        <v>1.386090811318139</v>
+        <v>1.111731069652548</v>
       </c>
       <c r="K19" t="n">
-        <v>1.303482191257356</v>
+        <v>1.121183310207803</v>
       </c>
       <c r="L19" t="n">
-        <v>1.247896422395008</v>
+        <v>1.129422438240957</v>
       </c>
       <c r="M19" t="n">
-        <v>1.200041001059512</v>
+        <v>1.141241406795019</v>
       </c>
       <c r="N19" t="n">
-        <v>1.176753615267698</v>
+        <v>1.151603317788136</v>
       </c>
       <c r="O19" t="n">
-        <v>1.165909825764475</v>
+        <v>1.160307413191936</v>
       </c>
       <c r="P19" t="n">
-        <v>1.169876689495289</v>
+        <v>1.163151525770992</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.18792710041819</v>
+        <v>1.159771696496589</v>
       </c>
       <c r="R19" t="n">
-        <v>1.188596970032813</v>
+        <v>1.154508879787832</v>
       </c>
       <c r="S19" t="n">
-        <v>1.191336116220388</v>
+        <v>1.147707478470175</v>
       </c>
       <c r="T19" t="n">
-        <v>1.19175986654552</v>
+        <v>1.1394155911994</v>
       </c>
       <c r="U19" t="n">
-        <v>1.197152475420558</v>
+        <v>1.128146766339508</v>
       </c>
       <c r="V19" t="n">
-        <v>1.197676060058681</v>
+        <v>1.123210256508858</v>
       </c>
       <c r="W19" t="n">
-        <v>1.19432020134685</v>
+        <v>1.120604371927175</v>
       </c>
       <c r="X19" t="n">
-        <v>1.189321030331141</v>
+        <v>1.123873603363842</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>1.129289253510071</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>1.133152148676627</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>1.135381982023709</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>1.137377236315926</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.33850711158389</v>
+        <v>0.8376776400682918</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5822649565019944</v>
+        <v>1.183987304395646</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6061917998494892</v>
+        <v>1.189634184651659</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7256733693098627</v>
+        <v>1.187003370327553</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8400188001113591</v>
+        <v>1.175282260700051</v>
       </c>
       <c r="F20" t="n">
-        <v>1.400337700712329</v>
+        <v>1.161065309258488</v>
       </c>
       <c r="G20" t="n">
-        <v>1.571329218969653</v>
+        <v>1.133955869599527</v>
       </c>
       <c r="H20" t="n">
-        <v>1.546004282237326</v>
+        <v>1.121783366063793</v>
       </c>
       <c r="I20" t="n">
-        <v>1.521673209097839</v>
+        <v>1.115868368667734</v>
       </c>
       <c r="J20" t="n">
-        <v>1.413548154398943</v>
+        <v>1.120022985360075</v>
       </c>
       <c r="K20" t="n">
-        <v>1.326771422249486</v>
+        <v>1.128719421895358</v>
       </c>
       <c r="L20" t="n">
-        <v>1.275443620869836</v>
+        <v>1.139538107329609</v>
       </c>
       <c r="M20" t="n">
-        <v>1.230545591879092</v>
+        <v>1.153360700720101</v>
       </c>
       <c r="N20" t="n">
-        <v>1.205220226362115</v>
+        <v>1.162423823099026</v>
       </c>
       <c r="O20" t="n">
-        <v>1.189014974233227</v>
+        <v>1.170121190728332</v>
       </c>
       <c r="P20" t="n">
-        <v>1.192511863891962</v>
+        <v>1.171936060282154</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.192303531179175</v>
+        <v>1.167411821859636</v>
       </c>
       <c r="R20" t="n">
-        <v>1.200806344289946</v>
+        <v>1.161659346322651</v>
       </c>
       <c r="S20" t="n">
-        <v>1.209216171578113</v>
+        <v>1.15448134378769</v>
       </c>
       <c r="T20" t="n">
-        <v>1.217350027755413</v>
+        <v>1.146144951504781</v>
       </c>
       <c r="U20" t="n">
-        <v>1.222834498145655</v>
+        <v>1.134395249320236</v>
       </c>
       <c r="V20" t="n">
-        <v>1.21961921798466</v>
+        <v>1.12935785847608</v>
       </c>
       <c r="W20" t="n">
-        <v>1.212493986011528</v>
+        <v>1.12682011868117</v>
       </c>
       <c r="X20" t="n">
-        <v>1.203606187802532</v>
+        <v>1.129890390471028</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>1.134925417662947</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>1.138337886036495</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>1.140205616738354</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>1.141721221346601</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>4.056898110222107</v>
+        <v>0.9426684551178852</v>
       </c>
       <c r="B21" t="n">
-        <v>0.6031128200078667</v>
+        <v>1.179016004865229</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6143730705602073</v>
+        <v>1.177623567516956</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7150542559143548</v>
+        <v>1.176885210292035</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8231906959059589</v>
+        <v>1.171402094927623</v>
       </c>
       <c r="F21" t="n">
-        <v>1.320984032712176</v>
+        <v>1.166621106343682</v>
       </c>
       <c r="G21" t="n">
-        <v>1.418867929842769</v>
+        <v>1.147886517787234</v>
       </c>
       <c r="H21" t="n">
-        <v>1.523769341008893</v>
+        <v>1.132054680731071</v>
       </c>
       <c r="I21" t="n">
-        <v>1.5044980602222</v>
+        <v>1.124203655519016</v>
       </c>
       <c r="J21" t="n">
-        <v>1.422812311575252</v>
+        <v>1.12956670397843</v>
       </c>
       <c r="K21" t="n">
-        <v>1.33262058113558</v>
+        <v>1.138983730374671</v>
       </c>
       <c r="L21" t="n">
-        <v>1.283376230580816</v>
+        <v>1.148628570467046</v>
       </c>
       <c r="M21" t="n">
-        <v>1.243739400438116</v>
+        <v>1.160703638975292</v>
       </c>
       <c r="N21" t="n">
-        <v>1.224801974517217</v>
+        <v>1.168196987206163</v>
       </c>
       <c r="O21" t="n">
-        <v>1.216673704759365</v>
+        <v>1.174763192217325</v>
       </c>
       <c r="P21" t="n">
-        <v>1.217798960776333</v>
+        <v>1.175547117580167</v>
       </c>
       <c r="Q21" t="n">
-        <v>1.216002010165363</v>
+        <v>1.169810072586711</v>
       </c>
       <c r="R21" t="n">
-        <v>1.221607932998828</v>
+        <v>1.163615358706248</v>
       </c>
       <c r="S21" t="n">
-        <v>1.226842812838376</v>
+        <v>1.156108341763058</v>
       </c>
       <c r="T21" t="n">
-        <v>1.231174531156896</v>
+        <v>1.147804380785428</v>
       </c>
       <c r="U21" t="n">
-        <v>1.233450357776266</v>
+        <v>1.135730922717243</v>
       </c>
       <c r="V21" t="n">
-        <v>1.226621206627292</v>
+        <v>1.130568496824373</v>
       </c>
       <c r="W21" t="n">
-        <v>1.219378310274172</v>
+        <v>1.12992600157822</v>
       </c>
       <c r="X21" t="n">
-        <v>1.213988250399756</v>
+        <v>1.130898161237379</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1.137607923718299</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>1.145520707743696</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>1.143547684514273</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>1.140939051865711</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4.929874859219733</v>
+        <v>1.060818355139448</v>
       </c>
       <c r="B22" t="n">
-        <v>0.6192838799512895</v>
+        <v>1.18641486487484</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6239924997553921</v>
+        <v>1.186451841621081</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7256752467859785</v>
+        <v>1.188227053929047</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8068673694838533</v>
+        <v>1.182169653333343</v>
       </c>
       <c r="F22" t="n">
-        <v>1.221179999057616</v>
+        <v>1.177022501087516</v>
       </c>
       <c r="G22" t="n">
-        <v>1.339695167205225</v>
+        <v>1.157924112831668</v>
       </c>
       <c r="H22" t="n">
-        <v>1.491813016741546</v>
+        <v>1.141323538617342</v>
       </c>
       <c r="I22" t="n">
-        <v>1.485411162398107</v>
+        <v>1.132790707168534</v>
       </c>
       <c r="J22" t="n">
-        <v>1.414429087927902</v>
+        <v>1.136899583036175</v>
       </c>
       <c r="K22" t="n">
-        <v>1.351158817253206</v>
+        <v>1.144420576773008</v>
       </c>
       <c r="L22" t="n">
-        <v>1.304521709005851</v>
+        <v>1.152758723378826</v>
       </c>
       <c r="M22" t="n">
-        <v>1.260859849192041</v>
+        <v>1.162975500350885</v>
       </c>
       <c r="N22" t="n">
-        <v>1.235312881978057</v>
+        <v>1.168773139313577</v>
       </c>
       <c r="O22" t="n">
-        <v>1.22815064406523</v>
+        <v>1.174155904088935</v>
       </c>
       <c r="P22" t="n">
-        <v>1.22778188118804</v>
+        <v>1.173845042852797</v>
       </c>
       <c r="Q22" t="n">
-        <v>1.224626540790994</v>
+        <v>1.166913382097778</v>
       </c>
       <c r="R22" t="n">
-        <v>1.227418816539331</v>
+        <v>1.160341542850565</v>
       </c>
       <c r="S22" t="n">
-        <v>1.232193818042563</v>
+        <v>1.152560030229165</v>
       </c>
       <c r="T22" t="n">
-        <v>1.241349785932082</v>
+        <v>1.144326086613849</v>
       </c>
       <c r="U22" t="n">
-        <v>1.247233386414085</v>
+        <v>1.135227734058869</v>
       </c>
       <c r="V22" t="n">
-        <v>1.243260822174596</v>
+        <v>1.135997565112853</v>
       </c>
       <c r="W22" t="n">
-        <v>1.235037712604593</v>
+        <v>1.14074244036605</v>
       </c>
       <c r="X22" t="n">
-        <v>1.226572296823456</v>
+        <v>1.143223097880037</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>1.151560371267562</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1.158979138399078</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>1.156818621669552</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>1.151653124281397</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5.990701631458083</v>
+        <v>1.193776641714436</v>
       </c>
       <c r="B23" t="n">
-        <v>0.6329100486851442</v>
+        <v>1.192991462081346</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6409929549058146</v>
+        <v>1.194256012695877</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7346418620309804</v>
+        <v>1.194214257799575</v>
       </c>
       <c r="E23" t="n">
-        <v>0.7918284619379792</v>
+        <v>1.187576670114921</v>
       </c>
       <c r="F23" t="n">
-        <v>1.10971974263281</v>
+        <v>1.182058625121739</v>
       </c>
       <c r="G23" t="n">
-        <v>1.264790064004544</v>
+        <v>1.162747268016652</v>
       </c>
       <c r="H23" t="n">
-        <v>1.456008416018452</v>
+        <v>1.145547745535437</v>
       </c>
       <c r="I23" t="n">
-        <v>1.472880441326446</v>
+        <v>1.136460292393445</v>
       </c>
       <c r="J23" t="n">
-        <v>1.42761227979386</v>
+        <v>1.139314387883053</v>
       </c>
       <c r="K23" t="n">
-        <v>1.362344154167912</v>
+        <v>1.144902192647208</v>
       </c>
       <c r="L23" t="n">
-        <v>1.316903160420491</v>
+        <v>1.151818657228509</v>
       </c>
       <c r="M23" t="n">
-        <v>1.275126253069772</v>
+        <v>1.160068477466518</v>
       </c>
       <c r="N23" t="n">
-        <v>1.254827340780085</v>
+        <v>1.164134755466172</v>
       </c>
       <c r="O23" t="n">
-        <v>1.244128292238781</v>
+        <v>1.168255105013577</v>
       </c>
       <c r="P23" t="n">
-        <v>1.243604946731161</v>
+        <v>1.166874657529899</v>
       </c>
       <c r="Q23" t="n">
-        <v>1.241853602790723</v>
+        <v>1.158743338568746</v>
       </c>
       <c r="R23" t="n">
-        <v>1.244983412010122</v>
+        <v>1.151836557651057</v>
       </c>
       <c r="S23" t="n">
-        <v>1.248430482743882</v>
+        <v>1.143876546305652</v>
       </c>
       <c r="T23" t="n">
-        <v>1.253402019557054</v>
+        <v>1.137110717748316</v>
       </c>
       <c r="U23" t="n">
-        <v>1.255655643915988</v>
+        <v>1.138756033581623</v>
       </c>
       <c r="V23" t="n">
-        <v>1.248263936321808</v>
+        <v>1.138604635874817</v>
       </c>
       <c r="W23" t="n">
-        <v>1.237045731720261</v>
+        <v>1.157154661739131</v>
       </c>
       <c r="X23" t="n">
-        <v>1.228303723394118</v>
+        <v>1.157876066535422</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>1.167927780462604</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>1.171939780441476</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>1.168566365104223</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>1.165215143297216</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>7.279800616041339</v>
+        <v>1.3433993325989</v>
       </c>
       <c r="B24" t="n">
-        <v>0.6487717369146283</v>
+        <v>1.197367815704774</v>
       </c>
       <c r="C24" t="n">
-        <v>0.6617444709617162</v>
+        <v>1.196509144638885</v>
       </c>
       <c r="D24" t="n">
-        <v>0.742268982499014</v>
+        <v>1.194693894836746</v>
       </c>
       <c r="E24" t="n">
-        <v>0.7787936956880466</v>
+        <v>1.187508445580391</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9966518393978288</v>
+        <v>1.181678168756626</v>
       </c>
       <c r="G24" t="n">
-        <v>1.203694251205987</v>
+        <v>1.162313174904742</v>
       </c>
       <c r="H24" t="n">
-        <v>1.407091607252132</v>
+        <v>1.144716933975659</v>
       </c>
       <c r="I24" t="n">
-        <v>1.446845701314532</v>
+        <v>1.135138679918511</v>
       </c>
       <c r="J24" t="n">
-        <v>1.426359246098177</v>
+        <v>1.136784413014974</v>
       </c>
       <c r="K24" t="n">
-        <v>1.359026691159617</v>
+        <v>1.140371258222603</v>
       </c>
       <c r="L24" t="n">
-        <v>1.320498507416272</v>
+        <v>1.1458630336099</v>
       </c>
       <c r="M24" t="n">
-        <v>1.281561729775348</v>
+        <v>1.154446293443167</v>
       </c>
       <c r="N24" t="n">
-        <v>1.264607428932041</v>
+        <v>1.160508732362338</v>
       </c>
       <c r="O24" t="n">
-        <v>1.254470076232183</v>
+        <v>1.166751936917282</v>
       </c>
       <c r="P24" t="n">
-        <v>1.252743637615122</v>
+        <v>1.166573028941739</v>
       </c>
       <c r="Q24" t="n">
-        <v>1.24964547562081</v>
+        <v>1.159280039752714</v>
       </c>
       <c r="R24" t="n">
-        <v>1.25464955375372</v>
+        <v>1.154649696492781</v>
       </c>
       <c r="S24" t="n">
-        <v>1.257385163414265</v>
+        <v>1.14772184221263</v>
       </c>
       <c r="T24" t="n">
-        <v>1.258761598535233</v>
+        <v>1.143776968582007</v>
       </c>
       <c r="U24" t="n">
-        <v>1.257718923893613</v>
+        <v>1.143334759406355</v>
       </c>
       <c r="V24" t="n">
-        <v>1.255708303403593</v>
+        <v>1.160973542913346</v>
       </c>
       <c r="W24" t="n">
-        <v>1.253558826255283</v>
+        <v>1.178764179147208</v>
       </c>
       <c r="X24" t="n">
-        <v>1.255924054041701</v>
+        <v>1.179302320484352</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>1.188794797322456</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>1.192517614425033</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>1.188942859707802</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>1.185315141120985</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>8.846292182376176</v>
+        <v>1.511775070615662</v>
       </c>
       <c r="B25" t="n">
-        <v>0.6665617470400719</v>
+        <v>1.196103251686285</v>
       </c>
       <c r="C25" t="n">
-        <v>0.684492774437492</v>
+        <v>1.193141591968686</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7476740071643168</v>
+        <v>1.18963952916959</v>
       </c>
       <c r="E25" t="n">
-        <v>0.7683510017027013</v>
+        <v>1.181948431796771</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9065040363289386</v>
+        <v>1.175860541389157</v>
       </c>
       <c r="G25" t="n">
-        <v>1.161510933963104</v>
+        <v>1.156622000229579</v>
       </c>
       <c r="H25" t="n">
-        <v>1.377439349713112</v>
+        <v>1.138800858755851</v>
       </c>
       <c r="I25" t="n">
-        <v>1.428662755588449</v>
+        <v>1.130328980007249</v>
       </c>
       <c r="J25" t="n">
-        <v>1.410353329513845</v>
+        <v>1.13790689333815</v>
       </c>
       <c r="K25" t="n">
-        <v>1.372130798861134</v>
+        <v>1.14653577297952</v>
       </c>
       <c r="L25" t="n">
-        <v>1.341591567698419</v>
+        <v>1.155215897361079</v>
       </c>
       <c r="M25" t="n">
-        <v>1.302158260164344</v>
+        <v>1.16372283912448</v>
       </c>
       <c r="N25" t="n">
-        <v>1.281512755082036</v>
+        <v>1.168197648093804</v>
       </c>
       <c r="O25" t="n">
-        <v>1.273680575027001</v>
+        <v>1.173250091998042</v>
       </c>
       <c r="P25" t="n">
-        <v>1.273389088343161</v>
+        <v>1.172118566677688</v>
       </c>
       <c r="Q25" t="n">
-        <v>1.268423566158708</v>
+        <v>1.163706760622923</v>
       </c>
       <c r="R25" t="n">
-        <v>1.258228674809165</v>
+        <v>1.158628732791995</v>
       </c>
       <c r="S25" t="n">
-        <v>1.258329300931825</v>
+        <v>1.151494114540578</v>
       </c>
       <c r="T25" t="n">
-        <v>1.265762763727346</v>
+        <v>1.149571956426775</v>
       </c>
       <c r="U25" t="n">
-        <v>1.268480135095224</v>
+        <v>1.149030364981519</v>
       </c>
       <c r="V25" t="n">
-        <v>1.274338688753094</v>
+        <v>1.1779659710665</v>
       </c>
       <c r="W25" t="n">
-        <v>1.271423966619209</v>
+        <v>1.194900936627022</v>
       </c>
       <c r="X25" t="n">
-        <v>1.27404913493052</v>
+        <v>1.195212552978702</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>1.204145371348114</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>1.207064644687605</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1.203315804581482</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>1.199239610526563</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10.74986658336873</v>
+        <v>1.701254279852589</v>
       </c>
       <c r="B26" t="n">
-        <v>0.6861000188777203</v>
+        <v>1.189246566732219</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7078306535510459</v>
+        <v>1.18422014858182</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7551457610520085</v>
+        <v>1.179114532397851</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7638873164203128</v>
+        <v>1.171055910700152</v>
       </c>
       <c r="F26" t="n">
-        <v>0.8448966741410749</v>
+        <v>1.164732763834144</v>
       </c>
       <c r="G26" t="n">
-        <v>1.112916729893857</v>
+        <v>1.149443437499086</v>
       </c>
       <c r="H26" t="n">
-        <v>1.348414874863399</v>
+        <v>1.141280722571479</v>
       </c>
       <c r="I26" t="n">
-        <v>1.415869812319574</v>
+        <v>1.140367036834131</v>
       </c>
       <c r="J26" t="n">
-        <v>1.403062767017791</v>
+        <v>1.14664505238108</v>
       </c>
       <c r="K26" t="n">
-        <v>1.380427434816738</v>
+        <v>1.153497877967671</v>
       </c>
       <c r="L26" t="n">
-        <v>1.348690483370202</v>
+        <v>1.160826451287476</v>
       </c>
       <c r="M26" t="n">
-        <v>1.314943457156184</v>
+        <v>1.167339111941965</v>
       </c>
       <c r="N26" t="n">
-        <v>1.308342776799534</v>
+        <v>1.170186897303935</v>
       </c>
       <c r="O26" t="n">
-        <v>1.29743062763564</v>
+        <v>1.173873285264458</v>
       </c>
       <c r="P26" t="n">
-        <v>1.294428619633061</v>
+        <v>1.171306640811426</v>
       </c>
       <c r="Q26" t="n">
-        <v>1.288012652281846</v>
+        <v>1.161836665629024</v>
       </c>
       <c r="R26" t="n">
-        <v>1.277212980198438</v>
+        <v>1.156376647693586</v>
       </c>
       <c r="S26" t="n">
-        <v>1.276293558222363</v>
+        <v>1.149670795209615</v>
       </c>
       <c r="T26" t="n">
-        <v>1.283127295898545</v>
+        <v>1.149754457850326</v>
       </c>
       <c r="U26" t="n">
-        <v>1.284175864013898</v>
+        <v>1.161011916679161</v>
       </c>
       <c r="V26" t="n">
-        <v>1.287008425988798</v>
+        <v>1.188036662753999</v>
       </c>
       <c r="W26" t="n">
-        <v>1.281717642529458</v>
+        <v>1.203528004437528</v>
       </c>
       <c r="X26" t="n">
-        <v>1.282331966791329</v>
+        <v>1.204726082551915</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>1.213659863917601</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>1.21872688749207</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>1.215763747622403</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>1.210450190937565</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>13.06305841790402</v>
+        <v>1.914481976169958</v>
       </c>
       <c r="B27" t="n">
-        <v>0.7073432854682573</v>
+        <v>1.184213015507979</v>
       </c>
       <c r="C27" t="n">
-        <v>0.731565508616778</v>
+        <v>1.178106296917764</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7665772961751181</v>
+        <v>1.172833206749134</v>
       </c>
       <c r="E27" t="n">
-        <v>0.7720857013641019</v>
+        <v>1.167351483451534</v>
       </c>
       <c r="F27" t="n">
-        <v>0.8370942413334365</v>
+        <v>1.16708787968515</v>
       </c>
       <c r="G27" t="n">
-        <v>1.075425713713885</v>
+        <v>1.155684133459868</v>
       </c>
       <c r="H27" t="n">
-        <v>1.307053789832961</v>
+        <v>1.146806556108372</v>
       </c>
       <c r="I27" t="n">
-        <v>1.389964907873145</v>
+        <v>1.144969425800036</v>
       </c>
       <c r="J27" t="n">
-        <v>1.402642436058869</v>
+        <v>1.149924055497075</v>
       </c>
       <c r="K27" t="n">
-        <v>1.375011521826795</v>
+        <v>1.154690718911348</v>
       </c>
       <c r="L27" t="n">
-        <v>1.369401154295283</v>
+        <v>1.160160706851001</v>
       </c>
       <c r="M27" t="n">
-        <v>1.337380974602899</v>
+        <v>1.163949280443059</v>
       </c>
       <c r="N27" t="n">
-        <v>1.319537796690055</v>
+        <v>1.164946066150083</v>
       </c>
       <c r="O27" t="n">
-        <v>1.306441565652856</v>
+        <v>1.169036635008922</v>
       </c>
       <c r="P27" t="n">
-        <v>1.308180733485981</v>
+        <v>1.167653688826139</v>
       </c>
       <c r="Q27" t="n">
-        <v>1.301807356709136</v>
+        <v>1.161397031427861</v>
       </c>
       <c r="R27" t="n">
-        <v>1.287635744783616</v>
+        <v>1.163350674145195</v>
       </c>
       <c r="S27" t="n">
-        <v>1.283736488107912</v>
+        <v>1.163502598969408</v>
       </c>
       <c r="T27" t="n">
-        <v>1.287609080606736</v>
+        <v>1.161489272617795</v>
       </c>
       <c r="U27" t="n">
-        <v>1.285928829165866</v>
+        <v>1.172079045410435</v>
       </c>
       <c r="V27" t="n">
-        <v>1.285610941137</v>
+        <v>1.198265477827871</v>
       </c>
       <c r="W27" t="n">
-        <v>1.287090147857773</v>
+        <v>1.212707613227237</v>
       </c>
       <c r="X27" t="n">
-        <v>1.293775810873848</v>
+        <v>1.215628403863848</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>1.224055196512707</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>1.228716757516029</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>1.225659795437027</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>1.220256840725881</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>15.874010519682</v>
+        <v>2.154434690031883</v>
       </c>
       <c r="B28" t="n">
-        <v>0.7299611290341214</v>
+        <v>1.189549089056559</v>
       </c>
       <c r="C28" t="n">
-        <v>0.7555347071744866</v>
+        <v>1.181794343708358</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7795445340940287</v>
+        <v>1.175175721560872</v>
       </c>
       <c r="E28" t="n">
-        <v>0.783342168021866</v>
+        <v>1.169028438087529</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8400346406313258</v>
+        <v>1.168047733649718</v>
       </c>
       <c r="G28" t="n">
-        <v>1.0651661385749</v>
+        <v>1.15633407482859</v>
       </c>
       <c r="H28" t="n">
-        <v>1.280564431639988</v>
+        <v>1.149498947744345</v>
       </c>
       <c r="I28" t="n">
-        <v>1.352253236584116</v>
+        <v>1.144440577049396</v>
       </c>
       <c r="J28" t="n">
-        <v>1.388726304808433</v>
+        <v>1.146980786709016</v>
       </c>
       <c r="K28" t="n">
-        <v>1.3943982502273</v>
+        <v>1.155510547026749</v>
       </c>
       <c r="L28" t="n">
-        <v>1.384085419728926</v>
+        <v>1.16216383002491</v>
       </c>
       <c r="M28" t="n">
-        <v>1.348263576060386</v>
+        <v>1.166429641408891</v>
       </c>
       <c r="N28" t="n">
-        <v>1.329530998837257</v>
+        <v>1.173907407381445</v>
       </c>
       <c r="O28" t="n">
-        <v>1.319260641856479</v>
+        <v>1.180089734332304</v>
       </c>
       <c r="P28" t="n">
-        <v>1.31513657531308</v>
+        <v>1.178924711256717</v>
       </c>
       <c r="Q28" t="n">
-        <v>1.305440244504519</v>
+        <v>1.175390451610322</v>
       </c>
       <c r="R28" t="n">
-        <v>1.292957808508759</v>
+        <v>1.1753975223124</v>
       </c>
       <c r="S28" t="n">
-        <v>1.292201566897673</v>
+        <v>1.174156793693123</v>
       </c>
       <c r="T28" t="n">
-        <v>1.29998930657871</v>
+        <v>1.176390089545959</v>
       </c>
       <c r="U28" t="n">
-        <v>1.302640022825268</v>
+        <v>1.180103819381714</v>
       </c>
       <c r="V28" t="n">
-        <v>1.306001891245047</v>
+        <v>1.205000221523058</v>
       </c>
       <c r="W28" t="n">
-        <v>1.304836660571758</v>
+        <v>1.218630444655109</v>
       </c>
       <c r="X28" t="n">
-        <v>1.309175448966696</v>
+        <v>1.221258019218532</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>1.229156809715683</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>1.233469356288608</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>1.230260792076804</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>1.224784880938677</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>19.28983258879171</v>
+        <v>2.424462017082328</v>
       </c>
       <c r="B29" t="n">
-        <v>0.75360056427168</v>
+        <v>1.188677052407523</v>
       </c>
       <c r="C29" t="n">
-        <v>0.779609954843645</v>
+        <v>1.179285876742002</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7933547011842396</v>
+        <v>1.171094070431258</v>
       </c>
       <c r="E29" t="n">
-        <v>0.7957384104033414</v>
+        <v>1.165691946775266</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8410688721418674</v>
+        <v>1.165661324365193</v>
       </c>
       <c r="G29" t="n">
-        <v>1.044744051326941</v>
+        <v>1.159948051494228</v>
       </c>
       <c r="H29" t="n">
-        <v>1.254662005457047</v>
+        <v>1.161853473594597</v>
       </c>
       <c r="I29" t="n">
-        <v>1.332922147243811</v>
+        <v>1.156839860124574</v>
       </c>
       <c r="J29" t="n">
-        <v>1.378364580231475</v>
+        <v>1.158662872702312</v>
       </c>
       <c r="K29" t="n">
-        <v>1.39994341234031</v>
+        <v>1.171327887973347</v>
       </c>
       <c r="L29" t="n">
-        <v>1.384190938932722</v>
+        <v>1.180228961127203</v>
       </c>
       <c r="M29" t="n">
-        <v>1.350557641811305</v>
+        <v>1.185461684322556</v>
       </c>
       <c r="N29" t="n">
-        <v>1.347769277839405</v>
+        <v>1.190349067960707</v>
       </c>
       <c r="O29" t="n">
-        <v>1.335225701038504</v>
+        <v>1.195390555856871</v>
       </c>
       <c r="P29" t="n">
-        <v>1.333696978513638</v>
+        <v>1.197511746263672</v>
       </c>
       <c r="Q29" t="n">
-        <v>1.325787853481834</v>
+        <v>1.19327663182389</v>
       </c>
       <c r="R29" t="n">
-        <v>1.311868740452884</v>
+        <v>1.192721569042727</v>
       </c>
       <c r="S29" t="n">
-        <v>1.308258216854641</v>
+        <v>1.19091129989419</v>
       </c>
       <c r="T29" t="n">
-        <v>1.312937177024421</v>
+        <v>1.192363102054693</v>
       </c>
       <c r="U29" t="n">
-        <v>1.312516356431023</v>
+        <v>1.19097315208253</v>
       </c>
       <c r="V29" t="n">
-        <v>1.312514557171414</v>
+        <v>1.217753910829601</v>
       </c>
       <c r="W29" t="n">
-        <v>1.308481754261335</v>
+        <v>1.233089661894894</v>
       </c>
       <c r="X29" t="n">
-        <v>1.310498805972291</v>
+        <v>1.234092720727106</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>1.242022544524903</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>1.244010819717247</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>1.240587929681831</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>1.237162397254126</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>23.44068254473251</v>
+        <v>2.728333376486768</v>
       </c>
       <c r="B30" t="n">
-        <v>0.7780557036689753</v>
+        <v>1.188534268186222</v>
       </c>
       <c r="C30" t="n">
-        <v>0.803698011665936</v>
+        <v>1.181615791584221</v>
       </c>
       <c r="D30" t="n">
-        <v>0.8080888428075467</v>
+        <v>1.175824081291782</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8094946695933901</v>
+        <v>1.171979655157566</v>
       </c>
       <c r="F30" t="n">
-        <v>0.8382313901219635</v>
+        <v>1.173094629087169</v>
       </c>
       <c r="G30" t="n">
-        <v>1.021503961295967</v>
+        <v>1.170270839557725</v>
       </c>
       <c r="H30" t="n">
-        <v>1.217870187010226</v>
+        <v>1.171533089356811</v>
       </c>
       <c r="I30" t="n">
-        <v>1.312541269002871</v>
+        <v>1.165596180888196</v>
       </c>
       <c r="J30" t="n">
-        <v>1.380648366126434</v>
+        <v>1.170443517355524</v>
       </c>
       <c r="K30" t="n">
-        <v>1.390992947933766</v>
+        <v>1.187597779154505</v>
       </c>
       <c r="L30" t="n">
-        <v>1.383623087782506</v>
+        <v>1.195887038110253</v>
       </c>
       <c r="M30" t="n">
-        <v>1.366784352086149</v>
+        <v>1.200582920551022</v>
       </c>
       <c r="N30" t="n">
-        <v>1.353324018906027</v>
+        <v>1.2050836230826</v>
       </c>
       <c r="O30" t="n">
-        <v>1.344390447641349</v>
+        <v>1.209626487371001</v>
       </c>
       <c r="P30" t="n">
-        <v>1.342840368084728</v>
+        <v>1.211312664110994</v>
       </c>
       <c r="Q30" t="n">
-        <v>1.333299945659777</v>
+        <v>1.206373068873697</v>
       </c>
       <c r="R30" t="n">
-        <v>1.316703058252157</v>
+        <v>1.205287486012326</v>
       </c>
       <c r="S30" t="n">
-        <v>1.310431089540738</v>
+        <v>1.202917078603827</v>
       </c>
       <c r="T30" t="n">
-        <v>1.31205400399789</v>
+        <v>1.203576869635819</v>
       </c>
       <c r="U30" t="n">
-        <v>1.308859181996017</v>
+        <v>1.203438796750054</v>
       </c>
       <c r="V30" t="n">
-        <v>1.305524708680467</v>
+        <v>1.230677154804948</v>
       </c>
       <c r="W30" t="n">
-        <v>1.298885535085359</v>
+        <v>1.245138361029362</v>
       </c>
       <c r="X30" t="n">
-        <v>1.298724200084312</v>
+        <v>1.245988924050257</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>1.253365858482315</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>1.255121546137839</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>1.251579478025873</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>1.24785726304635</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>28.48472611847307</v>
+        <v>3.07029062975785</v>
       </c>
       <c r="B31" t="n">
-        <v>0.8031886942317608</v>
+        <v>1.199257522640633</v>
       </c>
       <c r="C31" t="n">
-        <v>0.827755871339503</v>
+        <v>1.190507770895476</v>
       </c>
       <c r="D31" t="n">
-        <v>0.8240672219403299</v>
+        <v>1.183298859464546</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8241874361525668</v>
+        <v>1.178626667379684</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8382076864738517</v>
+        <v>1.178918778853576</v>
       </c>
       <c r="G31" t="n">
-        <v>0.9958230848516411</v>
+        <v>1.175448368294312</v>
       </c>
       <c r="H31" t="n">
-        <v>1.184492822218068</v>
+        <v>1.176047072717054</v>
       </c>
       <c r="I31" t="n">
-        <v>1.28170637492533</v>
+        <v>1.171407173706112</v>
       </c>
       <c r="J31" t="n">
-        <v>1.369518482776287</v>
+        <v>1.183449336316458</v>
       </c>
       <c r="K31" t="n">
-        <v>1.387667916798264</v>
+        <v>1.199219842512954</v>
       </c>
       <c r="L31" t="n">
-        <v>1.392714053008464</v>
+        <v>1.20681118315185</v>
       </c>
       <c r="M31" t="n">
-        <v>1.370614279201523</v>
+        <v>1.210870702723272</v>
       </c>
       <c r="N31" t="n">
-        <v>1.35148783424862</v>
+        <v>1.214968952495455</v>
       </c>
       <c r="O31" t="n">
-        <v>1.340841891766521</v>
+        <v>1.21894426580608</v>
       </c>
       <c r="P31" t="n">
-        <v>1.337672300948725</v>
+        <v>1.220140829207781</v>
       </c>
       <c r="Q31" t="n">
-        <v>1.326753896700366</v>
+        <v>1.214540436802042</v>
       </c>
       <c r="R31" t="n">
-        <v>1.308005337511314</v>
+        <v>1.212916709735268</v>
       </c>
       <c r="S31" t="n">
-        <v>1.300361865087146</v>
+        <v>1.210010616859346</v>
       </c>
       <c r="T31" t="n">
-        <v>1.300948325407112</v>
+        <v>1.209926166129633</v>
       </c>
       <c r="U31" t="n">
-        <v>1.296631462919849</v>
+        <v>1.212746709225597</v>
       </c>
       <c r="V31" t="n">
-        <v>1.294905612443612</v>
+        <v>1.238561233162929</v>
       </c>
       <c r="W31" t="n">
-        <v>1.292788286398718</v>
+        <v>1.252121615326693</v>
       </c>
       <c r="X31" t="n">
-        <v>1.300964522987506</v>
+        <v>1.252761255993112</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>1.259582555229087</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>1.261124054733027</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>1.257474227840281</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>1.253470353168443</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>34.61416366592753</v>
+        <v>3.455107294592218</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8289593031205306</v>
+        <v>1.20461487131721</v>
       </c>
       <c r="C32" t="n">
-        <v>0.8468122518281236</v>
+        <v>1.194119334133416</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8412446924533523</v>
+        <v>1.185612729374299</v>
       </c>
       <c r="E32" t="n">
-        <v>0.8400867013966087</v>
+        <v>1.181745154252925</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8528446270648823</v>
+        <v>1.185280964258018</v>
       </c>
       <c r="G32" t="n">
-        <v>0.988800826742978</v>
+        <v>1.186019761851929</v>
       </c>
       <c r="H32" t="n">
-        <v>1.166946228864612</v>
+        <v>1.189378841418138</v>
       </c>
       <c r="I32" t="n">
-        <v>1.269982513458222</v>
+        <v>1.185599782315161</v>
       </c>
       <c r="J32" t="n">
-        <v>1.354141105346834</v>
+        <v>1.191841374893504</v>
       </c>
       <c r="K32" t="n">
-        <v>1.390469812459058</v>
+        <v>1.206064938601264</v>
       </c>
       <c r="L32" t="n">
-        <v>1.388164496524209</v>
+        <v>1.212877843878471</v>
       </c>
       <c r="M32" t="n">
-        <v>1.36138875465069</v>
+        <v>1.21624982240195</v>
       </c>
       <c r="N32" t="n">
-        <v>1.337144879014366</v>
+        <v>1.219875416494807</v>
       </c>
       <c r="O32" t="n">
-        <v>1.330181692151736</v>
+        <v>1.223231112768655</v>
       </c>
       <c r="P32" t="n">
-        <v>1.32767456464391</v>
+        <v>1.223910491295277</v>
       </c>
       <c r="Q32" t="n">
-        <v>1.318275052072898</v>
+        <v>1.217737426906138</v>
       </c>
       <c r="R32" t="n">
-        <v>1.303265602005816</v>
+        <v>1.215542101742535</v>
       </c>
       <c r="S32" t="n">
-        <v>1.297399894248443</v>
+        <v>1.212142303000286</v>
       </c>
       <c r="T32" t="n">
-        <v>1.298689021217711</v>
+        <v>1.211313601410734</v>
       </c>
       <c r="U32" t="n">
-        <v>1.295444902868936</v>
+        <v>1.217040571919018</v>
       </c>
       <c r="V32" t="n">
-        <v>1.305802066183521</v>
+        <v>1.241358785761392</v>
       </c>
       <c r="W32" t="n">
-        <v>1.31496929077023</v>
+        <v>1.254012904325034</v>
       </c>
       <c r="X32" t="n">
-        <v>1.330355734673668</v>
+        <v>1.25448665671662</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1.260734786044695</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1.262022429244229</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1.258316524603289</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1.254063097821179</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>42.06255385108274</v>
+        <v>3.888155180308087</v>
       </c>
       <c r="B33" t="n">
-        <v>0.8550882679096548</v>
+        <v>1.209454822803015</v>
       </c>
       <c r="C33" t="n">
-        <v>0.8659468185896271</v>
+        <v>1.201772635626133</v>
       </c>
       <c r="D33" t="n">
-        <v>0.8594930970139444</v>
+        <v>1.196990252368349</v>
       </c>
       <c r="E33" t="n">
-        <v>0.8574451370808475</v>
+        <v>1.194114808337483</v>
       </c>
       <c r="F33" t="n">
-        <v>0.8686827714445668</v>
+        <v>1.197512732289522</v>
       </c>
       <c r="G33" t="n">
-        <v>0.9755717967240285</v>
+        <v>1.197636320409145</v>
       </c>
       <c r="H33" t="n">
-        <v>1.146058172248441</v>
+        <v>1.200257639300724</v>
       </c>
       <c r="I33" t="n">
-        <v>1.254745327338092</v>
+        <v>1.195574685904854</v>
       </c>
       <c r="J33" t="n">
-        <v>1.356883843552042</v>
+        <v>1.196328157387014</v>
       </c>
       <c r="K33" t="n">
-        <v>1.379828413334496</v>
+        <v>1.20827462643747</v>
       </c>
       <c r="L33" t="n">
-        <v>1.370660070235483</v>
+        <v>1.215703007296941</v>
       </c>
       <c r="M33" t="n">
-        <v>1.359742561216521</v>
+        <v>1.218729086061277</v>
       </c>
       <c r="N33" t="n">
-        <v>1.341014347568663</v>
+        <v>1.221964399166711</v>
       </c>
       <c r="O33" t="n">
-        <v>1.328810267977369</v>
+        <v>1.225192836968333</v>
       </c>
       <c r="P33" t="n">
-        <v>1.324634747995937</v>
+        <v>1.225661573986276</v>
       </c>
       <c r="Q33" t="n">
-        <v>1.313654931544562</v>
+        <v>1.219835432071803</v>
       </c>
       <c r="R33" t="n">
-        <v>1.297183129685344</v>
+        <v>1.220020525859028</v>
       </c>
       <c r="S33" t="n">
-        <v>1.299354250980783</v>
+        <v>1.219236551327666</v>
       </c>
       <c r="T33" t="n">
-        <v>1.306068168266776</v>
+        <v>1.220099513491601</v>
       </c>
       <c r="U33" t="n">
-        <v>1.31840754000979</v>
+        <v>1.227936596820066</v>
       </c>
       <c r="V33" t="n">
-        <v>1.329744881005493</v>
+        <v>1.245558537665821</v>
       </c>
       <c r="W33" t="n">
-        <v>1.337570445804336</v>
+        <v>1.2541391447452</v>
       </c>
       <c r="X33" t="n">
-        <v>1.351013742023821</v>
+        <v>1.253446150597471</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1.258866150397725</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>1.260379700464517</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>1.258267006081641</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>1.258018878835427</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>51.11371326347566</v>
+        <v>4.375479375074184</v>
       </c>
       <c r="B34" t="n">
-        <v>0.8815247141581661</v>
+        <v>1.220481351422624</v>
       </c>
       <c r="C34" t="n">
-        <v>0.88607680100016</v>
+        <v>1.211459473902471</v>
       </c>
       <c r="D34" t="n">
-        <v>0.8789365056340805</v>
+        <v>1.205746484727771</v>
       </c>
       <c r="E34" t="n">
-        <v>0.8760535588271272</v>
+        <v>1.202236904881661</v>
       </c>
       <c r="F34" t="n">
-        <v>0.8858791967148252</v>
+        <v>1.204799212480509</v>
       </c>
       <c r="G34" t="n">
-        <v>0.9637411929194406</v>
+        <v>1.204298296624807</v>
       </c>
       <c r="H34" t="n">
-        <v>1.130911413279604</v>
+        <v>1.206099543174874</v>
       </c>
       <c r="I34" t="n">
-        <v>1.238053141927721</v>
+        <v>1.200543731062405</v>
       </c>
       <c r="J34" t="n">
-        <v>1.347169084433506</v>
+        <v>1.202353510755273</v>
       </c>
       <c r="K34" t="n">
-        <v>1.358791348556397</v>
+        <v>1.212795165543388</v>
       </c>
       <c r="L34" t="n">
-        <v>1.370572595439602</v>
+        <v>1.222787739570933</v>
       </c>
       <c r="M34" t="n">
-        <v>1.362044167545572</v>
+        <v>1.228271593107332</v>
       </c>
       <c r="N34" t="n">
-        <v>1.340360713569854</v>
+        <v>1.23365137371478</v>
       </c>
       <c r="O34" t="n">
-        <v>1.32486676567994</v>
+        <v>1.238790528439964</v>
       </c>
       <c r="P34" t="n">
-        <v>1.329480238611381</v>
+        <v>1.242271015329298</v>
       </c>
       <c r="Q34" t="n">
-        <v>1.33032466951397</v>
+        <v>1.240052176399047</v>
       </c>
       <c r="R34" t="n">
-        <v>1.332248589678622</v>
+        <v>1.240145415274558</v>
       </c>
       <c r="S34" t="n">
-        <v>1.333909579868182</v>
+        <v>1.238708113149962</v>
       </c>
       <c r="T34" t="n">
-        <v>1.332505184232126</v>
+        <v>1.238872938247337</v>
       </c>
       <c r="U34" t="n">
-        <v>1.335727701133072</v>
+        <v>1.236636250674028</v>
       </c>
       <c r="V34" t="n">
-        <v>1.345400045899253</v>
+        <v>1.253358031899944</v>
       </c>
       <c r="W34" t="n">
-        <v>1.351872470840179</v>
+        <v>1.263775002877237</v>
       </c>
       <c r="X34" t="n">
-        <v>1.363549569010334</v>
+        <v>1.26366251937805</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>1.268662427440878</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>1.269874370697956</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>1.267290653750802</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>1.265403992766487</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>62.11253108478471</v>
+        <v>4.923882631706739</v>
       </c>
       <c r="B35" t="n">
-        <v>0.9082571931182486</v>
+        <v>1.226557745687834</v>
       </c>
       <c r="C35" t="n">
-        <v>0.9075004999319946</v>
+        <v>1.216212257971262</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8997201575163528</v>
+        <v>1.209625098232338</v>
       </c>
       <c r="E35" t="n">
-        <v>0.8960614146205961</v>
+        <v>1.205454733375947</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9049446300915864</v>
+        <v>1.207208359619677</v>
       </c>
       <c r="G35" t="n">
-        <v>0.9645681795836744</v>
+        <v>1.205968462283951</v>
       </c>
       <c r="H35" t="n">
-        <v>1.122532924125125</v>
+        <v>1.208684510389088</v>
       </c>
       <c r="I35" t="n">
-        <v>1.238626572342288</v>
+        <v>1.20779711124607</v>
       </c>
       <c r="J35" t="n">
-        <v>1.32625603333084</v>
+        <v>1.216683073750779</v>
       </c>
       <c r="K35" t="n">
-        <v>1.361395626583095</v>
+        <v>1.23232494703487</v>
       </c>
       <c r="L35" t="n">
-        <v>1.366047172004293</v>
+        <v>1.24149201950387</v>
       </c>
       <c r="M35" t="n">
-        <v>1.350935550905386</v>
+        <v>1.246187625918846</v>
       </c>
       <c r="N35" t="n">
-        <v>1.355998481095813</v>
+        <v>1.251089088475907</v>
       </c>
       <c r="O35" t="n">
-        <v>1.3669830368364</v>
+        <v>1.255604935371659</v>
       </c>
       <c r="P35" t="n">
-        <v>1.372020512489848</v>
+        <v>1.258483039797932</v>
       </c>
       <c r="Q35" t="n">
-        <v>1.370984274710169</v>
+        <v>1.255527168646844</v>
       </c>
       <c r="R35" t="n">
-        <v>1.371732243214822</v>
+        <v>1.254977745149489</v>
       </c>
       <c r="S35" t="n">
-        <v>1.373067015405855</v>
+        <v>1.252940688323769</v>
       </c>
       <c r="T35" t="n">
-        <v>1.372329040487372</v>
+        <v>1.252422185595971</v>
       </c>
       <c r="U35" t="n">
-        <v>1.370877275170251</v>
+        <v>1.254028766556094</v>
       </c>
       <c r="V35" t="n">
-        <v>1.368429176477941</v>
+        <v>1.261602480270498</v>
       </c>
       <c r="W35" t="n">
-        <v>1.363851821814592</v>
+        <v>1.269302605906418</v>
       </c>
       <c r="X35" t="n">
-        <v>1.373757982042346</v>
+        <v>1.269070449698482</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>1.273581732357536</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>1.277268662077284</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>1.277385209263373</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>1.278609485443407</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>75.47811089113596</v>
+        <v>5.541020330009492</v>
       </c>
       <c r="B36" t="n">
-        <v>0.9343959498367487</v>
+        <v>1.227668800320311</v>
       </c>
       <c r="C36" t="n">
-        <v>0.9302453584562347</v>
+        <v>1.216090819090197</v>
       </c>
       <c r="D36" t="n">
-        <v>0.9220200317337758</v>
+        <v>1.215994802091689</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9179799147025547</v>
+        <v>1.215847531418517</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9261326567431551</v>
+        <v>1.216791203860702</v>
       </c>
       <c r="G36" t="n">
-        <v>0.9661270544906367</v>
+        <v>1.217254669718226</v>
       </c>
       <c r="H36" t="n">
-        <v>1.118856789333295</v>
+        <v>1.218987185429052</v>
       </c>
       <c r="I36" t="n">
-        <v>1.229822095023408</v>
+        <v>1.220100779038813</v>
       </c>
       <c r="J36" t="n">
-        <v>1.327463085828595</v>
+        <v>1.232871425567355</v>
       </c>
       <c r="K36" t="n">
-        <v>1.351628423416549</v>
+        <v>1.246832714786375</v>
       </c>
       <c r="L36" t="n">
-        <v>1.348743147012251</v>
+        <v>1.254987660492354</v>
       </c>
       <c r="M36" t="n">
-        <v>1.370969169399027</v>
+        <v>1.258872355411275</v>
       </c>
       <c r="N36" t="n">
-        <v>1.403558753544899</v>
+        <v>1.263229454271917</v>
       </c>
       <c r="O36" t="n">
-        <v>1.413755365104792</v>
+        <v>1.267103146292411</v>
       </c>
       <c r="P36" t="n">
-        <v>1.416658197720241</v>
+        <v>1.269275055679496</v>
       </c>
       <c r="Q36" t="n">
-        <v>1.414126854807369</v>
+        <v>1.265608114982392</v>
       </c>
       <c r="R36" t="n">
-        <v>1.412470168712761</v>
+        <v>1.264379223707723</v>
       </c>
       <c r="S36" t="n">
-        <v>1.411945598658432</v>
+        <v>1.261756324219238</v>
       </c>
       <c r="T36" t="n">
-        <v>1.41012578013465</v>
+        <v>1.261589521102773</v>
       </c>
       <c r="U36" t="n">
-        <v>1.407433104808431</v>
+        <v>1.269631445047213</v>
       </c>
       <c r="V36" t="n">
-        <v>1.404770894795954</v>
+        <v>1.276621592667912</v>
       </c>
       <c r="W36" t="n">
-        <v>1.400367083011321</v>
+        <v>1.280039662741139</v>
       </c>
       <c r="X36" t="n">
-        <v>1.397823262769053</v>
+        <v>1.279262507472187</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>1.285958989125682</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>1.290691906359591</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>1.290485417239599</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>1.291250893979732</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>91.7197403518815</v>
+        <v>6.235507341273912</v>
       </c>
       <c r="B37" t="n">
-        <v>0.9592951391980931</v>
+        <v>1.235180378884447</v>
       </c>
       <c r="C37" t="n">
-        <v>0.9545361586748</v>
+        <v>1.235708027398654</v>
       </c>
       <c r="D37" t="n">
-        <v>0.9460341449705891</v>
+        <v>1.23526288248042</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9419210970250315</v>
+        <v>1.234320969653802</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9494125737318408</v>
+        <v>1.234069315742655</v>
       </c>
       <c r="G37" t="n">
-        <v>0.9743046274826833</v>
+        <v>1.231311264288734</v>
       </c>
       <c r="H37" t="n">
-        <v>1.123792378462206</v>
+        <v>1.231836551572929</v>
       </c>
       <c r="I37" t="n">
-        <v>1.224921511661525</v>
+        <v>1.232904577877524</v>
       </c>
       <c r="J37" t="n">
-        <v>1.319758804190131</v>
+        <v>1.243948318938837</v>
       </c>
       <c r="K37" t="n">
-        <v>1.332520316586751</v>
+        <v>1.25613210294127</v>
       </c>
       <c r="L37" t="n">
-        <v>1.363701569649193</v>
+        <v>1.263265333000441</v>
       </c>
       <c r="M37" t="n">
-        <v>1.412201476320371</v>
+        <v>1.266246968384772</v>
       </c>
       <c r="N37" t="n">
-        <v>1.446909293330402</v>
+        <v>1.269933807442108</v>
       </c>
       <c r="O37" t="n">
-        <v>1.45827630312665</v>
+        <v>1.273101173508128</v>
       </c>
       <c r="P37" t="n">
-        <v>1.462399362527599</v>
+        <v>1.274594969544173</v>
       </c>
       <c r="Q37" t="n">
-        <v>1.459850833488912</v>
+        <v>1.2701608001652</v>
       </c>
       <c r="R37" t="n">
-        <v>1.457908773940093</v>
+        <v>1.26829903400219</v>
       </c>
       <c r="S37" t="n">
-        <v>1.456811179020757</v>
+        <v>1.265625195447202</v>
       </c>
       <c r="T37" t="n">
-        <v>1.453682070210661</v>
+        <v>1.273216675411047</v>
       </c>
       <c r="U37" t="n">
-        <v>1.451394863855191</v>
+        <v>1.280678054762302</v>
       </c>
       <c r="V37" t="n">
-        <v>1.449936379881725</v>
+        <v>1.287070317725604</v>
       </c>
       <c r="W37" t="n">
-        <v>1.447356241864943</v>
+        <v>1.290120144765136</v>
       </c>
       <c r="X37" t="n">
-        <v>1.444292115270852</v>
+        <v>1.28908550127414</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>1.295308032726454</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>1.299478113627511</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>1.298980983940474</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>1.299219750175777</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>111.4562973409621</v>
+        <v>7.017038286703826</v>
       </c>
       <c r="B38" t="n">
-        <v>0.9857712159436908</v>
+        <v>1.251832654601652</v>
       </c>
       <c r="C38" t="n">
-        <v>0.9806286842423396</v>
+        <v>1.251223173506777</v>
       </c>
       <c r="D38" t="n">
-        <v>0.971995049383965</v>
+        <v>1.249513402035925</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9679757084264382</v>
+        <v>1.247465310707103</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9750824154632822</v>
+        <v>1.246105116737334</v>
       </c>
       <c r="G38" t="n">
-        <v>0.9997795335231452</v>
+        <v>1.241925350984029</v>
       </c>
       <c r="H38" t="n">
-        <v>1.123914415650748</v>
+        <v>1.242420088581322</v>
       </c>
       <c r="I38" t="n">
-        <v>1.230123093051145</v>
+        <v>1.244979837158276</v>
       </c>
       <c r="J38" t="n">
-        <v>1.303817805626896</v>
+        <v>1.254913691594411</v>
       </c>
       <c r="K38" t="n">
-        <v>1.348742608264176</v>
+        <v>1.26500053204109</v>
       </c>
       <c r="L38" t="n">
-        <v>1.407721870528938</v>
+        <v>1.27190694445573</v>
       </c>
       <c r="M38" t="n">
-        <v>1.4660798195602</v>
+        <v>1.273499428928443</v>
       </c>
       <c r="N38" t="n">
-        <v>1.499407601737097</v>
+        <v>1.276174206771857</v>
       </c>
       <c r="O38" t="n">
-        <v>1.508599795936428</v>
+        <v>1.278524024608996</v>
       </c>
       <c r="P38" t="n">
-        <v>1.509107621250408</v>
+        <v>1.279251857258922</v>
       </c>
       <c r="Q38" t="n">
-        <v>1.503865111107207</v>
+        <v>1.274732282346691</v>
       </c>
       <c r="R38" t="n">
-        <v>1.499688408758681</v>
+        <v>1.272856294791854</v>
       </c>
       <c r="S38" t="n">
-        <v>1.497072370969505</v>
+        <v>1.272578965562145</v>
       </c>
       <c r="T38" t="n">
-        <v>1.493361858473725</v>
+        <v>1.2801661036862</v>
       </c>
       <c r="U38" t="n">
-        <v>1.489798432098704</v>
+        <v>1.287037502067073</v>
       </c>
       <c r="V38" t="n">
-        <v>1.486945354108386</v>
+        <v>1.292788707948317</v>
       </c>
       <c r="W38" t="n">
-        <v>1.483677660679896</v>
+        <v>1.295443079898539</v>
       </c>
       <c r="X38" t="n">
-        <v>1.480966799848935</v>
+        <v>1.294211918865996</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>1.299918876621245</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>1.303507694572887</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>1.302740146836804</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>1.302466809635852</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>135.4398319194775</v>
+        <v>7.896522868499725</v>
       </c>
       <c r="B39" t="n">
-        <v>1.014126954835973</v>
+        <v>1.26307284139637</v>
       </c>
       <c r="C39" t="n">
-        <v>1.008782706744576</v>
+        <v>1.2612384930054</v>
       </c>
       <c r="D39" t="n">
-        <v>1.000414276444761</v>
+        <v>1.258294508591555</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9964551979393145</v>
+        <v>1.255142821784734</v>
       </c>
       <c r="F39" t="n">
-        <v>1.003842272729249</v>
+        <v>1.254045425304212</v>
       </c>
       <c r="G39" t="n">
-        <v>1.028272838159487</v>
+        <v>1.251410447441889</v>
       </c>
       <c r="H39" t="n">
-        <v>1.139935616140639</v>
+        <v>1.252866091094007</v>
       </c>
       <c r="I39" t="n">
-        <v>1.232398797694279</v>
+        <v>1.253996824598349</v>
       </c>
       <c r="J39" t="n">
-        <v>1.326749309897334</v>
+        <v>1.26219917776487</v>
       </c>
       <c r="K39" t="n">
-        <v>1.395992842082888</v>
+        <v>1.270418710209507</v>
       </c>
       <c r="L39" t="n">
-        <v>1.456290294113878</v>
+        <v>1.276098761218282</v>
       </c>
       <c r="M39" t="n">
-        <v>1.510324839350304</v>
+        <v>1.276542544787669</v>
       </c>
       <c r="N39" t="n">
-        <v>1.539933445500735</v>
+        <v>1.27841504132609</v>
       </c>
       <c r="O39" t="n">
-        <v>1.547055271612666</v>
+        <v>1.279999074110744</v>
       </c>
       <c r="P39" t="n">
-        <v>1.547323733476213</v>
+        <v>1.279976366623213</v>
       </c>
       <c r="Q39" t="n">
-        <v>1.542576069978461</v>
+        <v>1.277315737327681</v>
       </c>
       <c r="R39" t="n">
-        <v>1.538660431505909</v>
+        <v>1.276493092904744</v>
       </c>
       <c r="S39" t="n">
-        <v>1.535840107123851</v>
+        <v>1.275326041606432</v>
       </c>
       <c r="T39" t="n">
-        <v>1.531923793498849</v>
+        <v>1.282477233301216</v>
       </c>
       <c r="U39" t="n">
-        <v>1.528109429162168</v>
+        <v>1.289364070365675</v>
       </c>
       <c r="V39" t="n">
-        <v>1.525508548926753</v>
+        <v>1.293681803431352</v>
       </c>
       <c r="W39" t="n">
-        <v>1.522756858163639</v>
+        <v>1.29686050630308</v>
       </c>
       <c r="X39" t="n">
-        <v>1.51910047288965</v>
+        <v>1.297299428096638</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>1.304504789694263</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>1.309622449923661</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>1.30986364497066</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>1.310464705606874</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>164.5842227672371</v>
+        <v>8.886238162743403</v>
       </c>
       <c r="B40" t="n">
-        <v>1.044664542519751</v>
+        <v>1.274389720962046</v>
       </c>
       <c r="C40" t="n">
-        <v>1.039320232056478</v>
+        <v>1.271283081381618</v>
       </c>
       <c r="D40" t="n">
-        <v>1.031501724346462</v>
+        <v>1.266849293250162</v>
       </c>
       <c r="E40" t="n">
-        <v>1.028155394469229</v>
+        <v>1.263490863916625</v>
       </c>
       <c r="F40" t="n">
-        <v>1.035948875019931</v>
+        <v>1.261897841207789</v>
       </c>
       <c r="G40" t="n">
-        <v>1.060872641748554</v>
+        <v>1.258073749708673</v>
       </c>
       <c r="H40" t="n">
-        <v>1.147611161569412</v>
+        <v>1.258235099529513</v>
       </c>
       <c r="I40" t="n">
-        <v>1.265535484549485</v>
+        <v>1.257978951550959</v>
       </c>
       <c r="J40" t="n">
-        <v>1.370846664477632</v>
+        <v>1.264429867705116</v>
       </c>
       <c r="K40" t="n">
-        <v>1.438104424119631</v>
+        <v>1.270800009388759</v>
       </c>
       <c r="L40" t="n">
-        <v>1.493982356048151</v>
+        <v>1.277510348765137</v>
       </c>
       <c r="M40" t="n">
-        <v>1.547601597923817</v>
+        <v>1.280690820775297</v>
       </c>
       <c r="N40" t="n">
-        <v>1.578950227144206</v>
+        <v>1.284554140237104</v>
       </c>
       <c r="O40" t="n">
-        <v>1.586733559015816</v>
+        <v>1.288110105546795</v>
       </c>
       <c r="P40" t="n">
-        <v>1.584962508629436</v>
+        <v>1.290657775297452</v>
       </c>
       <c r="Q40" t="n">
-        <v>1.578110254074669</v>
+        <v>1.288107426033167</v>
       </c>
       <c r="R40" t="n">
-        <v>1.571846479430281</v>
+        <v>1.28657799496251</v>
       </c>
       <c r="S40" t="n">
-        <v>1.567131320233643</v>
+        <v>1.290922073936039</v>
       </c>
       <c r="T40" t="n">
-        <v>1.561427995136302</v>
+        <v>1.29837166896496</v>
       </c>
       <c r="U40" t="n">
-        <v>1.556502548992077</v>
+        <v>1.304779022600245</v>
       </c>
       <c r="V40" t="n">
-        <v>1.552715104247772</v>
+        <v>1.308664651650614</v>
       </c>
       <c r="W40" t="n">
-        <v>1.549120811576417</v>
+        <v>1.311488300466365</v>
       </c>
       <c r="X40" t="n">
-        <v>1.544324563958531</v>
+        <v>1.31166302295655</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>1.318398239419108</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>1.323014633904444</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>1.32301483986378</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>1.323208496104102</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="B41" t="n">
-        <v>1.077787162836153</v>
+        <v>1.280932074494937</v>
       </c>
       <c r="C41" t="n">
-        <v>1.07259900831196</v>
+        <v>1.276600674983235</v>
       </c>
       <c r="D41" t="n">
-        <v>1.065585126482899</v>
+        <v>1.271214990779706</v>
       </c>
       <c r="E41" t="n">
-        <v>1.063106486010273</v>
+        <v>1.267001926606958</v>
       </c>
       <c r="F41" t="n">
-        <v>1.07155137006365</v>
+        <v>1.264508954486358</v>
       </c>
       <c r="G41" t="n">
-        <v>1.092894326152565</v>
+        <v>1.260985260087039</v>
       </c>
       <c r="H41" t="n">
-        <v>1.179348223113787</v>
+        <v>1.260713316584</v>
       </c>
       <c r="I41" t="n">
-        <v>1.299170252611759</v>
+        <v>1.26421607159064</v>
       </c>
       <c r="J41" t="n">
-        <v>1.408261300426335</v>
+        <v>1.273714804466333</v>
       </c>
       <c r="K41" t="n">
-        <v>1.472866689375812</v>
+        <v>1.283098626733785</v>
       </c>
       <c r="L41" t="n">
-        <v>1.532965357693897</v>
+        <v>1.290179564019575</v>
       </c>
       <c r="M41" t="n">
-        <v>1.583861090999128</v>
+        <v>1.29164186557303</v>
       </c>
       <c r="N41" t="n">
-        <v>1.60884562106973</v>
+        <v>1.294168897201698</v>
       </c>
       <c r="O41" t="n">
-        <v>1.613165428220062</v>
+        <v>1.296665646886092</v>
       </c>
       <c r="P41" t="n">
-        <v>1.608394360982573</v>
+        <v>1.298261133548261</v>
       </c>
       <c r="Q41" t="n">
-        <v>1.599635154761329</v>
+        <v>1.295337974305905</v>
       </c>
       <c r="R41" t="n">
-        <v>1.591127272284792</v>
+        <v>1.296223847749052</v>
       </c>
       <c r="S41" t="n">
-        <v>1.586985407368316</v>
+        <v>1.302810842583097</v>
       </c>
       <c r="T41" t="n">
-        <v>1.582088317745554</v>
+        <v>1.309853590285184</v>
       </c>
       <c r="U41" t="n">
-        <v>1.578519651492512</v>
+        <v>1.315768155448683</v>
       </c>
       <c r="V41" t="n">
-        <v>1.576958549198814</v>
+        <v>1.319111094500189</v>
       </c>
       <c r="W41" t="n">
-        <v>1.575708069585624</v>
+        <v>1.321607114168225</v>
       </c>
       <c r="X41" t="n">
-        <v>1.572563138427549</v>
+        <v>1.321582991040208</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>1.327828756688675</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>1.331888974193437</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>1.331631578812869</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>1.331433485534402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>